<commit_message>
added customer sites and login system for employees
</commit_message>
<xml_diff>
--- a/plans/scrum-planering.xlsx
+++ b/plans/scrum-planering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\2024\yrkesprov\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB698DE1-1A3E-4CA2-8817-18D2FDA3BECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC79C9F1-7823-45D3-A799-0C198C50BD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{41C2E65D-138E-4665-8AB5-B482A8FDA31A}"/>
   </bookViews>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="107">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -301,9 +301,6 @@
     <t>Stories / Uppgifter</t>
   </si>
   <si>
-    <t>Sökfunktionalitet</t>
-  </si>
-  <si>
     <t>Inmatningsfunktionalitet</t>
   </si>
   <si>
@@ -440,6 +437,18 @@
   </si>
   <si>
     <t>Sidan laddas till en extern server och fungerar</t>
+  </si>
+  <si>
+    <t>Skapa olika branches för kund, sökande samt admin</t>
+  </si>
+  <si>
+    <t>Kundfunktionalitet</t>
+  </si>
+  <si>
+    <t>Skapa kund sidorna</t>
+  </si>
+  <si>
+    <t>Alla sidor som kunden kommer till är skapade</t>
   </si>
 </sst>
 </file>
@@ -821,7 +830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="242">
+  <cellXfs count="253">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -831,12 +840,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1039,12 +1042,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1278,9 +1275,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1418,53 +1412,99 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1662,7 +1702,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1716,7 +1756,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1770,7 +1810,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2303,8 +2343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393BB06C-F8B0-4B23-ABA1-344E8BDDC048}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2317,247 +2357,247 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="223"/>
-      <c r="B1" s="228" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" s="227"/>
-      <c r="D1" s="227"/>
-      <c r="E1" s="227"/>
-      <c r="F1" s="226"/>
+      <c r="A1" s="218"/>
+      <c r="B1" s="234" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="236"/>
     </row>
     <row r="2" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A2" s="223"/>
-      <c r="B2" s="225" t="s">
+      <c r="A2" s="218"/>
+      <c r="B2" s="220" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="223" t="s">
+      <c r="E2" s="218" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="224"/>
+      <c r="F2" s="219"/>
     </row>
     <row r="3" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="223"/>
-      <c r="B3" s="221" t="s">
+      <c r="A3" s="218"/>
+      <c r="B3" s="216" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="222" t="s">
+      <c r="C3" s="217" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="221"/>
-      <c r="E3" s="221" t="s">
+      <c r="D3" s="216"/>
+      <c r="E3" s="216" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="212"/>
+      <c r="F3" s="207"/>
     </row>
     <row r="4" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="202">
+      <c r="A4" s="197">
         <v>1</v>
       </c>
-      <c r="B4" s="219" t="s">
+      <c r="B4" s="214" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="214">
+      <c r="C4" s="209">
         <v>8</v>
       </c>
-      <c r="D4" s="202">
+      <c r="D4" s="197">
         <v>1</v>
       </c>
-      <c r="E4" s="213" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="212"/>
-      <c r="I4" s="220"/>
+      <c r="E4" s="208" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="207"/>
+      <c r="I4" s="215"/>
     </row>
     <row r="5" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="202">
+      <c r="A5" s="197">
         <v>2</v>
       </c>
-      <c r="B5" s="219" t="s">
+      <c r="B5" s="214" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="214">
+      <c r="C5" s="209">
         <v>5</v>
       </c>
-      <c r="D5" s="202">
+      <c r="D5" s="197">
         <v>2</v>
       </c>
-      <c r="E5" s="213" t="s">
+      <c r="E5" s="208" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="212"/>
+      <c r="F5" s="207"/>
     </row>
     <row r="6" spans="1:9" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="202">
+      <c r="A6" s="197">
         <v>3</v>
       </c>
-      <c r="B6" s="219" t="s">
+      <c r="B6" s="210" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="209">
+        <v>14</v>
+      </c>
+      <c r="D6" s="197">
+        <v>3</v>
+      </c>
+      <c r="E6" s="213" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="207"/>
+    </row>
+    <row r="7" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="197">
+        <v>4</v>
+      </c>
+      <c r="B7" s="211" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="214">
-        <v>10</v>
-      </c>
-      <c r="D6" s="202">
+      <c r="C7" s="209">
+        <v>7</v>
+      </c>
+      <c r="D7" s="197">
+        <v>4</v>
+      </c>
+      <c r="E7" s="212" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="207"/>
+    </row>
+    <row r="8" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="197">
+        <v>5</v>
+      </c>
+      <c r="B8" s="211" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="209">
+        <v>6</v>
+      </c>
+      <c r="D8" s="197">
+        <v>8</v>
+      </c>
+      <c r="E8" s="208" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="207"/>
+    </row>
+    <row r="9" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="197">
+        <v>6</v>
+      </c>
+      <c r="B9" s="211" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="73">
+        <v>2</v>
+      </c>
+      <c r="D9" s="197">
+        <v>5</v>
+      </c>
+      <c r="E9" s="208" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="207"/>
+    </row>
+    <row r="10" spans="1:9" ht="57.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="197">
+        <v>7</v>
+      </c>
+      <c r="B10" s="210" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="209">
+        <v>2</v>
+      </c>
+      <c r="D10" s="197">
+        <v>7</v>
+      </c>
+      <c r="E10" s="208" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="207"/>
+    </row>
+    <row r="11" spans="1:9" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="197">
+        <v>8</v>
+      </c>
+      <c r="B11" s="208" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="209">
         <v>3</v>
       </c>
-      <c r="E6" s="218" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="212"/>
-    </row>
-    <row r="7" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="202">
-        <v>4</v>
-      </c>
-      <c r="B7" s="216" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="214">
-        <v>7</v>
-      </c>
-      <c r="D7" s="202">
-        <v>4</v>
-      </c>
-      <c r="E7" s="217" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="212"/>
-    </row>
-    <row r="8" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="202">
-        <v>5</v>
-      </c>
-      <c r="B8" s="216" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="214">
+      <c r="D11" s="197">
         <v>6</v>
       </c>
-      <c r="D8" s="202">
-        <v>8</v>
-      </c>
-      <c r="E8" s="213" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="212"/>
-    </row>
-    <row r="9" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="202">
-        <v>6</v>
-      </c>
-      <c r="B9" s="216" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="75">
-        <v>2</v>
-      </c>
-      <c r="D9" s="202">
-        <v>5</v>
-      </c>
-      <c r="E9" s="213" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="212"/>
-    </row>
-    <row r="10" spans="1:9" ht="57.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="202">
-        <v>7</v>
-      </c>
-      <c r="B10" s="215" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="214">
-        <v>2</v>
-      </c>
-      <c r="D10" s="202">
-        <v>6</v>
-      </c>
-      <c r="E10" s="213" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="212"/>
-    </row>
-    <row r="11" spans="1:9" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="202">
-        <v>8</v>
-      </c>
-      <c r="B11" s="213" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="214">
+      <c r="E11" s="208" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="207"/>
+    </row>
+    <row r="12" spans="1:9" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="197">
+        <v>9</v>
+      </c>
+      <c r="B12" s="210" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="209">
         <v>3</v>
       </c>
-      <c r="D11" s="202">
-        <v>7</v>
-      </c>
-      <c r="E11" s="213" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="212"/>
-    </row>
-    <row r="12" spans="1:9" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="202">
+      <c r="D12" s="197">
         <v>9</v>
       </c>
-      <c r="B12" s="215" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="214">
-        <v>3</v>
-      </c>
-      <c r="D12" s="202">
-        <v>9</v>
-      </c>
-      <c r="E12" s="213" t="s">
+      <c r="E12" s="208" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="212"/>
+      <c r="F12" s="207"/>
     </row>
     <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="207"/>
-      <c r="B13" s="211"/>
-      <c r="C13" s="204"/>
-      <c r="D13" s="204"/>
-      <c r="E13" s="210"/>
-      <c r="F13" s="203"/>
+      <c r="A13" s="202"/>
+      <c r="B13" s="206"/>
+      <c r="C13" s="199"/>
+      <c r="D13" s="199"/>
+      <c r="E13" s="205"/>
+      <c r="F13" s="198"/>
     </row>
     <row r="14" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="207"/>
-      <c r="B14" s="210"/>
-      <c r="C14" s="210"/>
-      <c r="D14" s="210"/>
-      <c r="E14" s="210"/>
-      <c r="F14" s="203"/>
+      <c r="A14" s="202"/>
+      <c r="B14" s="205"/>
+      <c r="C14" s="205"/>
+      <c r="D14" s="205"/>
+      <c r="E14" s="205"/>
+      <c r="F14" s="198"/>
     </row>
     <row r="15" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="209"/>
-      <c r="B15" s="210"/>
-      <c r="C15" s="209"/>
-      <c r="D15" s="209"/>
-      <c r="E15" s="208"/>
-      <c r="F15" s="203"/>
+      <c r="A15" s="204"/>
+      <c r="B15" s="205"/>
+      <c r="C15" s="204"/>
+      <c r="D15" s="204"/>
+      <c r="E15" s="203"/>
+      <c r="F15" s="198"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="207"/>
-      <c r="B16" s="206" t="s">
+      <c r="A16" s="202"/>
+      <c r="B16" s="201" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="205">
+      <c r="C16" s="200">
         <f>SUM(C4:C15)</f>
-        <v>46</v>
-      </c>
-      <c r="D16" s="204"/>
-      <c r="E16" s="204">
+        <v>50</v>
+      </c>
+      <c r="D16" s="199"/>
+      <c r="E16" s="199">
         <f>C16*60</f>
-        <v>2760</v>
-      </c>
-      <c r="F16" s="203"/>
+        <v>3000</v>
+      </c>
+      <c r="F16" s="198"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2580,8 +2620,8 @@
   <cols>
     <col min="1" max="1" width="6.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28" style="75" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="75" customWidth="1"/>
+    <col min="3" max="3" width="28" style="73" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="73" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" style="1" customWidth="1"/>
@@ -2596,370 +2636,370 @@
         <v>0</v>
       </c>
       <c r="D1" s="3"/>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="237" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="5"/>
+      <c r="H1" s="238"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="19"/>
-    </row>
-    <row r="4" spans="1:22" s="31" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="21" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="17"/>
+    </row>
+    <row r="4" spans="1:22" s="29" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="B4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="30"/>
+      <c r="K4" s="28"/>
     </row>
     <row r="5" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="35" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="36"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="19"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:22" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="41">
+      <c r="A6" s="38"/>
+      <c r="B6" s="39">
         <v>1</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="43">
+      <c r="D6" s="41">
         <f>SUM(D7:D13) / 60</f>
         <v>7.75</v>
       </c>
-      <c r="E6" s="240">
+      <c r="E6" s="232">
         <f>SUM(E7:E13)/60</f>
         <v>13.25</v>
       </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="8"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:22" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="51" t="s">
+      <c r="A7" s="38"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="52">
+      <c r="D7" s="50">
         <v>90</v>
       </c>
-      <c r="E7" s="53">
+      <c r="E7" s="51">
         <v>90</v>
       </c>
-      <c r="F7" s="54"/>
-      <c r="G7" s="55" t="s">
+      <c r="F7" s="52"/>
+      <c r="G7" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="56">
+      <c r="H7" s="54">
         <v>45604</v>
       </c>
-      <c r="I7" s="229" t="s">
+      <c r="I7" s="221" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" s="56"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:22" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="50">
+        <v>90</v>
+      </c>
+      <c r="E8" s="51">
+        <v>300</v>
+      </c>
+      <c r="F8" s="52"/>
+      <c r="G8" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="54">
+        <v>45608</v>
+      </c>
+      <c r="I8" s="221" t="s">
         <v>65</v>
       </c>
-      <c r="J7" s="58"/>
-      <c r="K7" s="8"/>
-    </row>
-    <row r="8" spans="1:22" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="51" t="s">
+      <c r="J8" s="56"/>
+      <c r="K8" s="57" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="50">
+        <v>30</v>
+      </c>
+      <c r="E9" s="51">
         <v>15</v>
       </c>
-      <c r="D8" s="52">
+      <c r="F9" s="52"/>
+      <c r="G9" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="54">
+        <v>45607</v>
+      </c>
+      <c r="I9" s="221" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="56"/>
+      <c r="K9" s="59" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="61.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="50">
+        <v>75</v>
+      </c>
+      <c r="E10" s="51">
+        <v>60</v>
+      </c>
+      <c r="F10" s="52"/>
+      <c r="G10" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="54">
+        <v>45607</v>
+      </c>
+      <c r="I10" s="221" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" s="56"/>
+      <c r="K10" s="61"/>
+    </row>
+    <row r="11" spans="1:22" ht="61.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="50">
+        <v>60</v>
+      </c>
+      <c r="E11" s="51">
+        <v>120</v>
+      </c>
+      <c r="F11" s="52"/>
+      <c r="G11" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="54">
+        <v>45609</v>
+      </c>
+      <c r="I11" s="221" t="s">
+        <v>68</v>
+      </c>
+      <c r="J11" s="231"/>
+      <c r="K11" s="62"/>
+    </row>
+    <row r="12" spans="1:22" ht="61.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="50">
+        <v>60</v>
+      </c>
+      <c r="E12" s="51">
+        <v>120</v>
+      </c>
+      <c r="F12" s="52"/>
+      <c r="G12" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="54">
+        <v>45610</v>
+      </c>
+      <c r="I12" s="221" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="56"/>
+      <c r="K12" s="62"/>
+    </row>
+    <row r="13" spans="1:22" ht="61.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="50">
+        <v>60</v>
+      </c>
+      <c r="E13" s="51">
         <v>90</v>
       </c>
-      <c r="E8" s="53">
-        <v>300</v>
-      </c>
-      <c r="F8" s="54"/>
-      <c r="G8" s="55" t="s">
+      <c r="F13" s="52"/>
+      <c r="G13" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="56">
-        <v>45608</v>
-      </c>
-      <c r="I8" s="229" t="s">
-        <v>66</v>
-      </c>
-      <c r="J8" s="58"/>
-      <c r="K8" s="59" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="60" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="52">
-        <v>30</v>
-      </c>
-      <c r="E9" s="53">
-        <v>15</v>
-      </c>
-      <c r="F9" s="54"/>
-      <c r="G9" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="56">
+      <c r="H13" s="54">
         <v>45607</v>
       </c>
-      <c r="I9" s="229" t="s">
-        <v>67</v>
-      </c>
-      <c r="J9" s="58"/>
-      <c r="K9" s="61" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="61.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="52">
-        <v>75</v>
-      </c>
-      <c r="E10" s="53">
-        <v>60</v>
-      </c>
-      <c r="F10" s="54"/>
-      <c r="G10" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="56">
-        <v>45607</v>
-      </c>
-      <c r="I10" s="229" t="s">
-        <v>68</v>
-      </c>
-      <c r="J10" s="58"/>
-      <c r="K10" s="63"/>
-    </row>
-    <row r="11" spans="1:22" ht="61.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="52">
-        <v>60</v>
-      </c>
-      <c r="E11" s="53">
-        <v>120</v>
-      </c>
-      <c r="F11" s="54"/>
-      <c r="G11" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="56">
-        <v>45609</v>
-      </c>
-      <c r="I11" s="229" t="s">
+      <c r="I13" s="221" t="s">
         <v>69</v>
       </c>
-      <c r="J11" s="239"/>
-      <c r="K11" s="64"/>
-    </row>
-    <row r="12" spans="1:22" ht="61.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="60" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="52">
-        <v>60</v>
-      </c>
-      <c r="E12" s="53">
-        <v>120</v>
-      </c>
-      <c r="F12" s="54"/>
-      <c r="G12" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="56">
-        <v>45610</v>
-      </c>
-      <c r="I12" s="229" t="s">
-        <v>64</v>
-      </c>
-      <c r="J12" s="58"/>
-      <c r="K12" s="64"/>
-    </row>
-    <row r="13" spans="1:22" ht="61.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="60" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="52">
-        <v>60</v>
-      </c>
-      <c r="E13" s="53">
-        <v>90</v>
-      </c>
-      <c r="F13" s="54"/>
-      <c r="G13" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="56">
-        <v>45607</v>
-      </c>
-      <c r="I13" s="229" t="s">
-        <v>70</v>
-      </c>
-      <c r="J13" s="58"/>
-      <c r="K13" s="64"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="62"/>
     </row>
     <row r="14" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="19"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="17"/>
     </row>
     <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="66"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="72"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="70"/>
     </row>
     <row r="16" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="19"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="17"/>
     </row>
     <row r="17" spans="2:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="66"/>
-      <c r="C17" s="67" t="s">
+      <c r="B17" s="64"/>
+      <c r="C17" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="67">
+      <c r="D17" s="65">
         <f>SUM(D7:D13)/60</f>
         <v>7.75</v>
       </c>
-      <c r="E17" s="73">
+      <c r="E17" s="71">
         <f>E6</f>
         <v>13.25</v>
       </c>
-      <c r="F17" s="69"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="70"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="74"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="72"/>
     </row>
     <row r="18" spans="2:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="66"/>
-      <c r="C18" s="67" t="s">
+      <c r="B18" s="64"/>
+      <c r="C18" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="67">
+      <c r="D18" s="65">
         <f>SUM(D17+D19)</f>
         <v>10</v>
       </c>
-      <c r="E18" s="67"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="74"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="72"/>
     </row>
     <row r="19" spans="2:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="66"/>
-      <c r="C19" s="67" t="s">
+      <c r="B19" s="64"/>
+      <c r="C19" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="67">
+      <c r="D19" s="65">
         <v>2.25</v>
       </c>
-      <c r="E19" s="67"/>
-      <c r="F19" s="69"/>
-      <c r="G19" s="70"/>
-      <c r="H19" s="70"/>
-      <c r="I19" s="71"/>
-      <c r="J19" s="49"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2976,8 +3016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF3BD90-0203-44B4-AE4B-CE188AD45574}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2996,386 +3036,424 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="76"/>
-      <c r="D1" s="77"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="75"/>
+      <c r="G1" s="237"/>
+      <c r="H1" s="237"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="19"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="17"/>
     </row>
     <row r="4" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="21" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="19"/>
+      <c r="K4" s="17"/>
     </row>
     <row r="5" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="19"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="242"/>
+      <c r="D5" s="242"/>
+      <c r="E5" s="243"/>
+      <c r="F5" s="243"/>
+      <c r="G5" s="244"/>
+      <c r="H5" s="245"/>
+      <c r="I5" s="243"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:22" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="82">
+      <c r="A6" s="38"/>
+      <c r="B6" s="241">
         <v>2</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="247" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="248">
+        <f>SUM(D7:D11)/60</f>
+        <v>3.5</v>
+      </c>
+      <c r="E6" s="136">
+        <f>SUM(E7:E11)/60</f>
+        <v>3</v>
+      </c>
+      <c r="F6" s="136"/>
+      <c r="G6" s="249"/>
+      <c r="H6" s="139"/>
+      <c r="I6" s="141"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:22" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="82" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="83">
+        <v>60</v>
+      </c>
+      <c r="E7" s="84">
+        <v>90</v>
+      </c>
+      <c r="F7" s="85"/>
+      <c r="G7" s="86" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="246">
+        <v>45610</v>
+      </c>
+      <c r="I7" s="87" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="84">
-        <f>SUM(D7:D12)/60</f>
-        <v>5.5</v>
-      </c>
-      <c r="E6" s="82">
-        <f>SUM(E7:E12)</f>
-        <v>90</v>
-      </c>
-      <c r="F6" s="82"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:22" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="85"/>
-      <c r="C7" s="86" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="87">
+      <c r="J7" s="6"/>
+      <c r="K7" s="88"/>
+    </row>
+    <row r="8" spans="1:22" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="89" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="90">
+        <v>30</v>
+      </c>
+      <c r="E8" s="91">
+        <v>30</v>
+      </c>
+      <c r="F8" s="85"/>
+      <c r="G8" s="86" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="54">
+        <v>45610</v>
+      </c>
+      <c r="I8" s="87" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8" s="56"/>
+      <c r="K8" s="88"/>
+    </row>
+    <row r="9" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="92" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="93">
+        <v>30</v>
+      </c>
+      <c r="E9" s="94">
+        <v>15</v>
+      </c>
+      <c r="F9" s="95"/>
+      <c r="G9" s="96" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="97">
+        <v>45611</v>
+      </c>
+      <c r="I9" s="98" t="s">
+        <v>103</v>
+      </c>
+      <c r="J9" s="99"/>
+      <c r="K9" s="17"/>
+    </row>
+    <row r="10" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="100"/>
+      <c r="C10" s="101" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="102">
+        <v>30</v>
+      </c>
+      <c r="E10" s="103">
+        <v>15</v>
+      </c>
+      <c r="F10" s="104"/>
+      <c r="G10" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="97">
+        <v>45611</v>
+      </c>
+      <c r="I10" s="194" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" s="104"/>
+      <c r="K10" s="17"/>
+    </row>
+    <row r="11" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="100"/>
+      <c r="C11" s="106" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="102">
         <v>60</v>
       </c>
-      <c r="E7" s="88">
-        <v>90</v>
-      </c>
-      <c r="F7" s="89"/>
-      <c r="G7" s="90" t="s">
+      <c r="E11" s="103">
+        <v>30</v>
+      </c>
+      <c r="F11" s="104"/>
+      <c r="G11" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="56">
+      <c r="H11" s="54">
         <v>45610</v>
       </c>
-      <c r="I7" s="91" t="s">
-        <v>72</v>
-      </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="92"/>
-    </row>
-    <row r="8" spans="1:22" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="85"/>
-      <c r="C8" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="94">
-        <v>30</v>
-      </c>
-      <c r="E8" s="95"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="90"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="91" t="s">
-        <v>73</v>
-      </c>
-      <c r="J8" s="58"/>
-      <c r="K8" s="92"/>
-    </row>
-    <row r="9" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="85"/>
-      <c r="C9" s="96" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="97">
-        <v>30</v>
-      </c>
-      <c r="E9" s="98"/>
-      <c r="F9" s="99"/>
-      <c r="G9" s="100"/>
-      <c r="H9" s="101"/>
-      <c r="I9" s="102"/>
-      <c r="J9" s="103"/>
-      <c r="K9" s="19"/>
-    </row>
-    <row r="10" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="104"/>
-      <c r="C10" s="105" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="106">
-        <v>30</v>
-      </c>
-      <c r="E10" s="107"/>
-      <c r="F10" s="108"/>
-      <c r="G10" s="109"/>
-      <c r="H10" s="101"/>
-      <c r="I10" s="199" t="s">
+      <c r="I11" s="194" t="s">
         <v>74</v>
       </c>
-      <c r="J10" s="108"/>
-      <c r="K10" s="19"/>
-    </row>
-    <row r="11" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="104"/>
-      <c r="C11" s="110" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="106">
+      <c r="J11" s="104"/>
+      <c r="K11" s="17"/>
+    </row>
+    <row r="12" spans="1:22" ht="46.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="113">
+        <v>3</v>
+      </c>
+      <c r="C12" s="114" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="114">
+        <f>SUM(D13:D17)/60</f>
+        <v>14</v>
+      </c>
+      <c r="E12" s="239">
+        <f>SUM(E13:E17)/60</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="115"/>
+      <c r="G12" s="116"/>
+      <c r="H12" s="117"/>
+      <c r="I12" s="118"/>
+      <c r="J12" s="119"/>
+      <c r="K12" s="17"/>
+    </row>
+    <row r="13" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="104"/>
+      <c r="C13" s="215" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="109">
+        <v>120</v>
+      </c>
+      <c r="E13" s="122">
         <v>60</v>
       </c>
-      <c r="E11" s="107"/>
-      <c r="F11" s="108"/>
-      <c r="G11" s="90"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="199" t="s">
+      <c r="F13" s="122"/>
+      <c r="G13" s="252" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="124">
+        <v>45611</v>
+      </c>
+      <c r="I13" s="215" t="s">
+        <v>106</v>
+      </c>
+      <c r="J13" s="104"/>
+      <c r="K13" s="17"/>
+    </row>
+    <row r="14" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="104"/>
+      <c r="C14" s="120" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="121">
+        <v>240</v>
+      </c>
+      <c r="E14" s="122"/>
+      <c r="F14" s="122"/>
+      <c r="G14" s="123"/>
+      <c r="H14" s="124"/>
+      <c r="I14" s="125" t="s">
+        <v>80</v>
+      </c>
+      <c r="J14" s="104"/>
+      <c r="K14" s="17"/>
+    </row>
+    <row r="15" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="104"/>
+      <c r="C15" s="120" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="121">
+        <v>180</v>
+      </c>
+      <c r="E15" s="73"/>
+      <c r="F15" s="122"/>
+      <c r="G15" s="123"/>
+      <c r="H15" s="124"/>
+      <c r="I15" s="125" t="s">
+        <v>79</v>
+      </c>
+      <c r="J15" s="112"/>
+      <c r="K15" s="17"/>
+    </row>
+    <row r="16" spans="1:22" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="104"/>
+      <c r="C16" s="102" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="102">
+        <v>180</v>
+      </c>
+      <c r="E16" s="103"/>
+      <c r="F16" s="104"/>
+      <c r="G16" s="105"/>
+      <c r="H16" s="126"/>
+      <c r="I16" s="194" t="s">
+        <v>82</v>
+      </c>
+      <c r="J16" s="104"/>
+      <c r="K16" s="17"/>
+    </row>
+    <row r="17" spans="1:11" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="107"/>
+      <c r="C17" s="108" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="109">
+        <v>120</v>
+      </c>
+      <c r="E17" s="110"/>
+      <c r="F17" s="107"/>
+      <c r="G17" s="111"/>
+      <c r="H17" s="97"/>
+      <c r="I17" s="112" t="s">
         <v>75</v>
       </c>
-      <c r="J11" s="108"/>
-      <c r="K11" s="19"/>
-    </row>
-    <row r="12" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="111"/>
-      <c r="C12" s="112" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="113">
-        <v>120</v>
-      </c>
-      <c r="E12" s="114"/>
-      <c r="F12" s="111"/>
-      <c r="G12" s="115"/>
-      <c r="H12" s="101"/>
-      <c r="I12" s="116" t="s">
-        <v>76</v>
-      </c>
-      <c r="J12" s="116"/>
-      <c r="K12" s="9"/>
-    </row>
-    <row r="13" spans="1:22" ht="46.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="117">
-        <v>3</v>
-      </c>
-      <c r="C13" s="118" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="118">
-        <f>SUM(D14:D17)/60</f>
-        <v>10</v>
-      </c>
-      <c r="E13" s="119">
-        <f>SUM(E14:E17)</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="119"/>
-      <c r="G13" s="120"/>
-      <c r="H13" s="121"/>
-      <c r="I13" s="122"/>
-      <c r="J13" s="123"/>
-      <c r="K13" s="19"/>
-    </row>
-    <row r="14" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="108"/>
-      <c r="C14" s="124" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" s="125">
-        <v>240</v>
-      </c>
-      <c r="E14" s="126"/>
-      <c r="F14" s="126"/>
-      <c r="G14" s="127"/>
-      <c r="H14" s="128"/>
-      <c r="I14" s="129" t="s">
-        <v>81</v>
-      </c>
-      <c r="J14" s="108"/>
-      <c r="K14" s="19"/>
-    </row>
-    <row r="15" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="108"/>
-      <c r="C15" s="124" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" s="125">
-        <v>180</v>
-      </c>
-      <c r="E15" s="75"/>
-      <c r="F15" s="126"/>
-      <c r="G15" s="127"/>
-      <c r="H15" s="128"/>
-      <c r="I15" s="129" t="s">
-        <v>80</v>
-      </c>
-      <c r="J15" s="116"/>
-      <c r="K15" s="19"/>
-    </row>
-    <row r="16" spans="1:22" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="108"/>
-      <c r="C16" s="106" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" s="106">
-        <v>180</v>
-      </c>
-      <c r="E16" s="107"/>
-      <c r="F16" s="108"/>
-      <c r="G16" s="109"/>
-      <c r="H16" s="130"/>
-      <c r="I16" s="199" t="s">
-        <v>83</v>
-      </c>
-      <c r="J16" s="108"/>
-      <c r="K16" s="19"/>
-    </row>
-    <row r="17" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="111"/>
-      <c r="C17" s="131"/>
-      <c r="D17" s="131"/>
-      <c r="E17" s="114"/>
-      <c r="F17" s="111"/>
-      <c r="G17" s="115"/>
-      <c r="H17" s="130"/>
-      <c r="I17" s="116"/>
-      <c r="J17" s="116"/>
-      <c r="K17" s="9"/>
+      <c r="J17" s="112"/>
+      <c r="K17" s="7"/>
     </row>
     <row r="18" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
-      <c r="B18" s="132"/>
-      <c r="C18" s="133" t="s">
+      <c r="A18" s="38"/>
+      <c r="B18" s="128"/>
+      <c r="C18" s="129" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="134">
-        <f>SUM(D6+D13)</f>
-        <v>15.5</v>
-      </c>
-      <c r="E18" s="134">
-        <f>SUM((E6+E13)/60)</f>
-        <v>1.5</v>
-      </c>
-      <c r="F18" s="68"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="70"/>
-      <c r="J18" s="72"/>
+      <c r="D18" s="130">
+        <f>SUM(D6+D12)</f>
+        <v>17.5</v>
+      </c>
+      <c r="E18" s="71">
+        <f>SUM((E6+E12))</f>
+        <v>4</v>
+      </c>
+      <c r="F18" s="66"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="70"/>
     </row>
     <row r="19" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="135"/>
-      <c r="C19" s="82" t="s">
+      <c r="B19" s="131"/>
+      <c r="C19" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="44">
+      <c r="D19" s="42">
         <f>SUM(D20+D18)</f>
-        <v>18</v>
-      </c>
-      <c r="E19" s="136"/>
-      <c r="F19" s="137"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="138"/>
-      <c r="J19" s="74"/>
+        <v>20</v>
+      </c>
+      <c r="E19" s="132"/>
+      <c r="F19" s="133"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="134"/>
+      <c r="J19" s="72"/>
     </row>
     <row r="20" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="139"/>
-      <c r="C20" s="140" t="s">
+      <c r="B20" s="135"/>
+      <c r="C20" s="136" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="241">
+      <c r="D20" s="233">
         <v>2.5</v>
       </c>
-      <c r="E20" s="141"/>
-      <c r="F20" s="142"/>
-      <c r="G20" s="143"/>
-      <c r="H20" s="143"/>
-      <c r="I20" s="144"/>
-      <c r="J20" s="145"/>
+      <c r="E20" s="137"/>
+      <c r="F20" s="138"/>
+      <c r="G20" s="139"/>
+      <c r="H20" s="139"/>
+      <c r="I20" s="140"/>
+      <c r="J20" s="141"/>
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="146"/>
-      <c r="C21" s="147"/>
-      <c r="D21" s="147"/>
-      <c r="E21" s="148"/>
-      <c r="F21" s="149"/>
-      <c r="G21" s="150"/>
-      <c r="H21" s="150"/>
-      <c r="I21" s="151"/>
-      <c r="J21" s="152"/>
+      <c r="B21" s="142"/>
+      <c r="C21" s="143"/>
+      <c r="D21" s="143"/>
+      <c r="E21" s="144"/>
+      <c r="F21" s="145"/>
+      <c r="G21" s="146"/>
+      <c r="H21" s="146"/>
+      <c r="I21" s="147"/>
+      <c r="J21" s="148"/>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="153"/>
-      <c r="C22" s="147"/>
-      <c r="D22" s="147"/>
-      <c r="E22" s="148"/>
-      <c r="F22" s="149"/>
-      <c r="G22" s="150"/>
-      <c r="H22" s="150"/>
-      <c r="I22" s="151"/>
-      <c r="J22" s="152"/>
+      <c r="B22" s="149"/>
+      <c r="C22" s="143"/>
+      <c r="D22" s="143"/>
+      <c r="E22" s="144"/>
+      <c r="F22" s="145"/>
+      <c r="G22" s="146"/>
+      <c r="H22" s="146"/>
+      <c r="I22" s="147"/>
+      <c r="J22" s="148"/>
     </row>
     <row r="31" spans="1:11" ht="13.2" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -3390,10 +3468,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C94DF7-B35F-4481-A77A-5670F6E3A59A}">
-  <dimension ref="A1:V17"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3401,7 +3479,7 @@
     <col min="1" max="1" width="6.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="28" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="75" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="73" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.109375" style="1"/>
     <col min="7" max="7" width="21" style="1" customWidth="1"/>
@@ -3412,297 +3490,309 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="76"/>
+      <c r="C1" s="74"/>
       <c r="D1" s="3"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5"/>
+      <c r="G1" s="237"/>
+      <c r="H1" s="238"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="154"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="150"/>
     </row>
     <row r="4" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="21" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="155" t="s">
+      <c r="F4" s="151" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="19"/>
+      <c r="K4" s="17"/>
     </row>
     <row r="5" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="19"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:22" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="117">
+      <c r="A6" s="38"/>
+      <c r="B6" s="113">
         <v>4</v>
       </c>
-      <c r="C6" s="118" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="118">
+      <c r="C6" s="114" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="114">
         <f>SUM(D7:D9)/60</f>
         <v>7</v>
       </c>
-      <c r="E6" s="119"/>
-      <c r="F6" s="119"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="156"/>
-      <c r="I6" s="157"/>
-      <c r="J6" s="158"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="116"/>
+      <c r="H6" s="152"/>
+      <c r="I6" s="153"/>
+      <c r="J6" s="154"/>
     </row>
     <row r="7" spans="1:22" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="108"/>
-      <c r="C7" s="124" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="104"/>
+      <c r="C7" s="120" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="121">
+        <v>120</v>
+      </c>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="123"/>
+      <c r="H7" s="107"/>
+      <c r="I7" s="155" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="125">
+      <c r="J7" s="104"/>
+    </row>
+    <row r="8" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="104"/>
+      <c r="C8" s="120" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="121">
         <v>120</v>
       </c>
-      <c r="E7" s="126"/>
-      <c r="F7" s="126"/>
-      <c r="G7" s="127"/>
-      <c r="H7" s="111"/>
-      <c r="I7" s="159" t="s">
+      <c r="E8" s="122"/>
+      <c r="F8" s="122"/>
+      <c r="G8" s="123"/>
+      <c r="H8" s="107"/>
+      <c r="I8" s="155" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8" s="104"/>
+    </row>
+    <row r="9" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="104"/>
+      <c r="C9" s="156" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="121">
+        <v>180</v>
+      </c>
+      <c r="E9" s="122"/>
+      <c r="F9" s="122"/>
+      <c r="G9" s="107"/>
+      <c r="H9" s="107"/>
+      <c r="I9" s="155" t="s">
+        <v>89</v>
+      </c>
+      <c r="J9" s="104"/>
+    </row>
+    <row r="10" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="107"/>
+      <c r="C10" s="240"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="240"/>
+      <c r="F10" s="240"/>
+      <c r="G10" s="240"/>
+      <c r="H10" s="240"/>
+      <c r="I10" s="240"/>
+      <c r="J10" s="104"/>
+    </row>
+    <row r="11" spans="1:22" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="113">
+        <v>5</v>
+      </c>
+      <c r="C11" s="114" t="s">
         <v>86</v>
       </c>
-      <c r="J7" s="108"/>
-    </row>
-    <row r="8" spans="1:22" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="108"/>
-      <c r="C8" s="124" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" s="125">
+      <c r="D11" s="229">
+        <f>SUM(D12:D15)/60</f>
+        <v>6.5</v>
+      </c>
+      <c r="E11" s="115"/>
+      <c r="F11" s="115"/>
+      <c r="G11" s="157"/>
+      <c r="H11" s="157"/>
+      <c r="I11" s="153"/>
+      <c r="J11" s="119"/>
+    </row>
+    <row r="12" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="104"/>
+      <c r="C12" s="120" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="227">
+        <v>150</v>
+      </c>
+      <c r="E12" s="122"/>
+      <c r="F12" s="122"/>
+      <c r="G12" s="123"/>
+      <c r="H12" s="124"/>
+      <c r="I12" s="121" t="s">
+        <v>98</v>
+      </c>
+      <c r="J12" s="112"/>
+      <c r="K12" s="166"/>
+    </row>
+    <row r="13" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="158"/>
+      <c r="C13" s="159" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="160">
         <v>120</v>
       </c>
-      <c r="E8" s="126"/>
-      <c r="F8" s="126"/>
-      <c r="G8" s="127"/>
-      <c r="H8" s="111"/>
-      <c r="I8" s="159" t="s">
-        <v>89</v>
-      </c>
-      <c r="J8" s="108"/>
-    </row>
-    <row r="9" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="108"/>
-      <c r="C9" s="160" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" s="125">
-        <v>180</v>
-      </c>
-      <c r="E9" s="126"/>
-      <c r="F9" s="126"/>
-      <c r="G9" s="111"/>
-      <c r="H9" s="111"/>
-      <c r="I9" s="159" t="s">
-        <v>90</v>
-      </c>
-      <c r="J9" s="108"/>
-    </row>
-    <row r="10" spans="1:22" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="117">
-        <v>5</v>
-      </c>
-      <c r="C10" s="118" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" s="237">
-        <f>SUM(D11:D14)/60</f>
-        <v>6.5</v>
-      </c>
-      <c r="E10" s="119"/>
-      <c r="F10" s="119"/>
-      <c r="G10" s="161"/>
-      <c r="H10" s="161"/>
-      <c r="I10" s="157"/>
-      <c r="J10" s="123"/>
-    </row>
-    <row r="11" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="108"/>
-      <c r="C11" s="124" t="s">
-        <v>98</v>
-      </c>
-      <c r="D11" s="235">
-        <v>150</v>
-      </c>
-      <c r="E11" s="126"/>
-      <c r="F11" s="126"/>
-      <c r="G11" s="127"/>
-      <c r="H11" s="128"/>
-      <c r="I11" s="125" t="s">
-        <v>99</v>
-      </c>
-      <c r="J11" s="116"/>
-      <c r="K11" s="170"/>
-    </row>
-    <row r="12" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="162"/>
-      <c r="C12" s="163" t="s">
+      <c r="E13" s="161"/>
+      <c r="F13" s="161"/>
+      <c r="G13" s="162"/>
+      <c r="H13" s="163"/>
+      <c r="I13" s="164" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="164">
-        <v>120</v>
-      </c>
-      <c r="E12" s="165"/>
-      <c r="F12" s="165"/>
-      <c r="G12" s="166"/>
-      <c r="H12" s="167"/>
-      <c r="I12" s="168" t="s">
+      <c r="J13" s="165"/>
+      <c r="K13" s="226"/>
+    </row>
+    <row r="14" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="167"/>
+      <c r="C14" s="222" t="s">
         <v>93</v>
       </c>
-      <c r="J12" s="169"/>
-      <c r="K12" s="234"/>
-    </row>
-    <row r="13" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="171"/>
-      <c r="C13" s="230" t="s">
+      <c r="D14" s="228">
+        <v>60</v>
+      </c>
+      <c r="E14" s="168"/>
+      <c r="F14" s="168"/>
+      <c r="G14" s="169"/>
+      <c r="H14" s="170"/>
+      <c r="I14" s="223" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="236">
+      <c r="J14" s="171"/>
+      <c r="K14" s="17"/>
+    </row>
+    <row r="15" spans="1:22" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" s="107"/>
+      <c r="C15" s="224" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="127">
         <v>60</v>
       </c>
-      <c r="E13" s="172"/>
-      <c r="F13" s="172"/>
-      <c r="G13" s="173"/>
-      <c r="H13" s="174"/>
-      <c r="I13" s="231" t="s">
-        <v>95</v>
-      </c>
-      <c r="J13" s="175"/>
-      <c r="K13" s="19"/>
-    </row>
-    <row r="14" spans="1:22" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="111"/>
-      <c r="C14" s="232" t="s">
+      <c r="E15" s="107"/>
+      <c r="F15" s="107"/>
+      <c r="G15" s="103"/>
+      <c r="H15" s="104"/>
+      <c r="I15" s="225" t="s">
         <v>96</v>
       </c>
-      <c r="D14" s="131">
-        <v>60</v>
-      </c>
-      <c r="E14" s="111"/>
-      <c r="F14" s="111"/>
-      <c r="G14" s="107"/>
-      <c r="H14" s="108"/>
-      <c r="I14" s="233" t="s">
-        <v>97</v>
-      </c>
-      <c r="J14" s="116"/>
-      <c r="K14" s="9"/>
-    </row>
-    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="66"/>
-      <c r="C15" s="133" t="s">
+      <c r="J15" s="112"/>
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="64"/>
+      <c r="C16" s="129" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="67">
-        <f>SUM(D6+D10)</f>
+      <c r="D16" s="65">
+        <f>SUM(D6+D11)</f>
         <v>13.5</v>
       </c>
-      <c r="E15" s="73">
-        <f>SUM((E11+E7)/60)</f>
+      <c r="E16" s="71">
+        <f>SUM((E12+E7)/60)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="69"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="74"/>
-    </row>
-    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="66"/>
-      <c r="C16" s="67" t="s">
+      <c r="F16" s="67"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="72"/>
+    </row>
+    <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="64"/>
+      <c r="C17" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="67">
-        <f>SUM(D15+D17)</f>
+      <c r="D17" s="65">
+        <f>SUM(D16+D18)</f>
         <v>15</v>
       </c>
-      <c r="E16" s="67"/>
-      <c r="F16" s="69"/>
-      <c r="G16" s="70"/>
-      <c r="H16" s="70"/>
-      <c r="I16" s="71"/>
-      <c r="J16" s="74"/>
-    </row>
-    <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="66"/>
-      <c r="C17" s="67" t="s">
+      <c r="E17" s="65"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="72"/>
+    </row>
+    <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="64"/>
+      <c r="C18" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="67">
+      <c r="D18" s="65">
         <v>1.5</v>
       </c>
-      <c r="E17" s="67"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="70"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="49"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3719,8 +3809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA02060-17A8-4F90-AA70-CE39812F4F3A}">
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3728,7 +3818,7 @@
     <col min="1" max="1" width="6.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="28" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="75" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="73" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.109375" style="1"/>
     <col min="7" max="7" width="21" style="1" customWidth="1"/>
@@ -3739,304 +3829,304 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="76"/>
+      <c r="C1" s="74"/>
       <c r="D1" s="3"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5"/>
+      <c r="G1" s="237"/>
+      <c r="H1" s="238"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="154"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="150"/>
     </row>
     <row r="4" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="21" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="19"/>
+      <c r="K4" s="17"/>
     </row>
     <row r="5" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="19"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="242"/>
+      <c r="D5" s="242"/>
+      <c r="E5" s="243"/>
+      <c r="F5" s="243"/>
+      <c r="G5" s="244"/>
+      <c r="H5" s="245"/>
+      <c r="I5" s="243"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:22" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="82">
+      <c r="B6" s="241">
         <v>6</v>
       </c>
-      <c r="C6" s="176" t="s">
+      <c r="C6" s="250" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="43">
+      <c r="D6" s="251">
         <f>SUM(D7:D9)</f>
         <v>180</v>
       </c>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="72"/>
+      <c r="E6" s="136"/>
+      <c r="F6" s="136"/>
+      <c r="G6" s="249"/>
+      <c r="H6" s="139"/>
+      <c r="I6" s="141"/>
+      <c r="J6" s="70"/>
     </row>
     <row r="7" spans="1:22" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="177"/>
-      <c r="C7" s="178" t="s">
+      <c r="B7" s="172"/>
+      <c r="C7" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="88">
+      <c r="D7" s="84">
         <v>60</v>
       </c>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="179"/>
-      <c r="H7" s="180"/>
-      <c r="I7" s="181" t="s">
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="174"/>
+      <c r="H7" s="175"/>
+      <c r="I7" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="103"/>
+      <c r="J7" s="99"/>
     </row>
     <row r="8" spans="1:22" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="177"/>
-      <c r="C8" s="57" t="s">
+      <c r="B8" s="172"/>
+      <c r="C8" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="52">
+      <c r="D8" s="50">
         <v>60</v>
       </c>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="57" t="s">
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="J8" s="177"/>
+    </row>
+    <row r="9" spans="1:22" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="172"/>
+      <c r="C9" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="50">
+        <v>60</v>
+      </c>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="J8" s="182"/>
-    </row>
-    <row r="9" spans="1:22" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="177"/>
-      <c r="C9" s="57" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="52">
+      <c r="J9" s="16"/>
+    </row>
+    <row r="10" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="178">
+        <v>7</v>
+      </c>
+      <c r="C10" s="179" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="180">
         <v>60</v>
       </c>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="57" t="s">
+      <c r="E10" s="181"/>
+      <c r="F10" s="181"/>
+      <c r="G10" s="182"/>
+      <c r="H10" s="182"/>
+      <c r="I10" s="183"/>
+      <c r="J10" s="184"/>
+    </row>
+    <row r="11" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="185"/>
+      <c r="C11" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="50">
+        <v>60</v>
+      </c>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="J9" s="18"/>
-    </row>
-    <row r="10" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="183">
-        <v>7</v>
-      </c>
-      <c r="C10" s="184" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="185">
+      <c r="J11" s="99"/>
+    </row>
+    <row r="12" spans="1:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="178">
+        <v>8</v>
+      </c>
+      <c r="C12" s="186" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="187">
         <v>60</v>
       </c>
-      <c r="E10" s="186"/>
-      <c r="F10" s="186"/>
-      <c r="G10" s="187"/>
-      <c r="H10" s="187"/>
-      <c r="I10" s="188"/>
-      <c r="J10" s="189"/>
-    </row>
-    <row r="11" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="190"/>
-      <c r="C11" s="57" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="52">
+      <c r="E12" s="188"/>
+      <c r="F12" s="188"/>
+      <c r="G12" s="189"/>
+      <c r="H12" s="189"/>
+      <c r="I12" s="190"/>
+      <c r="J12" s="191"/>
+    </row>
+    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="104"/>
+      <c r="C13" s="192" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="110">
         <v>60</v>
       </c>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="57" t="s">
+      <c r="E13" s="193"/>
+      <c r="F13" s="193"/>
+      <c r="G13" s="104"/>
+      <c r="H13" s="104"/>
+      <c r="I13" s="230" t="s">
         <v>102</v>
       </c>
-      <c r="J11" s="103"/>
-    </row>
-    <row r="12" spans="1:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="183">
-        <v>8</v>
-      </c>
-      <c r="C12" s="191" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="192">
-        <v>60</v>
-      </c>
-      <c r="E12" s="193"/>
-      <c r="F12" s="193"/>
-      <c r="G12" s="194"/>
-      <c r="H12" s="194"/>
-      <c r="I12" s="195"/>
-      <c r="J12" s="196"/>
-    </row>
-    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="108"/>
-      <c r="C13" s="197" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="114">
-        <v>60</v>
-      </c>
-      <c r="E13" s="198"/>
-      <c r="F13" s="198"/>
-      <c r="G13" s="108"/>
-      <c r="H13" s="108"/>
-      <c r="I13" s="238" t="s">
-        <v>103</v>
-      </c>
-      <c r="J13" s="116"/>
+      <c r="J13" s="112"/>
     </row>
     <row r="14" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="161">
+      <c r="B14" s="157">
         <v>9</v>
       </c>
-      <c r="C14" s="200" t="s">
+      <c r="C14" s="195" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="120">
+      <c r="D14" s="116">
         <v>120</v>
       </c>
-      <c r="E14" s="161"/>
-      <c r="F14" s="161"/>
-      <c r="G14" s="201"/>
-      <c r="H14" s="123"/>
-      <c r="I14" s="158"/>
-      <c r="J14" s="158"/>
+      <c r="E14" s="157"/>
+      <c r="F14" s="157"/>
+      <c r="G14" s="196"/>
+      <c r="H14" s="119"/>
+      <c r="I14" s="154"/>
+      <c r="J14" s="154"/>
     </row>
     <row r="15" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B15" s="177"/>
-      <c r="C15" s="178" t="s">
+      <c r="B15" s="172"/>
+      <c r="C15" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="88">
+      <c r="D15" s="84">
         <v>120</v>
       </c>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89"/>
-      <c r="G15" s="179"/>
-      <c r="H15" s="180"/>
-      <c r="I15" s="181"/>
-      <c r="J15" s="103"/>
+      <c r="E15" s="85"/>
+      <c r="F15" s="85"/>
+      <c r="G15" s="174"/>
+      <c r="H15" s="175"/>
+      <c r="I15" s="176"/>
+      <c r="J15" s="99"/>
     </row>
     <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="177"/>
-      <c r="C16" s="94"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="94"/>
-      <c r="J16" s="182"/>
+      <c r="B16" s="172"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="90"/>
+      <c r="J16" s="177"/>
     </row>
     <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="66"/>
-      <c r="C17" s="133" t="s">
+      <c r="B17" s="64"/>
+      <c r="C17" s="129" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="67">
+      <c r="D17" s="65">
         <f>SUM(D6+D10+D12+D14)/60</f>
         <v>7</v>
       </c>
-      <c r="E17" s="73">
+      <c r="E17" s="71">
         <f>E13</f>
         <v>0</v>
       </c>
-      <c r="F17" s="69"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="70"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="74"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="72"/>
     </row>
     <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="66"/>
-      <c r="C18" s="67" t="s">
+      <c r="B18" s="64"/>
+      <c r="C18" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="133"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="74"/>
+      <c r="D18" s="129"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="72"/>
     </row>
     <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="66"/>
-      <c r="C19" s="67" t="s">
+      <c r="B19" s="64"/>
+      <c r="C19" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="69"/>
-      <c r="G19" s="70"/>
-      <c r="H19" s="70"/>
-      <c r="I19" s="71"/>
-      <c r="J19" s="49"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
final day commit, started work on book insertion system
</commit_message>
<xml_diff>
--- a/plans/scrum-planering.xlsx
+++ b/plans/scrum-planering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\2024\yrkesprov\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC79C9F1-7823-45D3-A799-0C198C50BD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A9448D-35CA-4BCA-AFAA-152E0A7432B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{41C2E65D-138E-4665-8AB5-B482A8FDA31A}"/>
   </bookViews>
@@ -830,7 +830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="253">
+  <cellXfs count="254">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1451,24 +1451,6 @@
     <xf numFmtId="165" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1505,6 +1487,27 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2358,13 +2361,13 @@
   <sheetData>
     <row r="1" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="218"/>
-      <c r="B1" s="234" t="s">
+      <c r="B1" s="247" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="235"/>
-      <c r="D1" s="235"/>
-      <c r="E1" s="235"/>
-      <c r="F1" s="236"/>
+      <c r="C1" s="248"/>
+      <c r="D1" s="248"/>
+      <c r="E1" s="248"/>
+      <c r="F1" s="249"/>
     </row>
     <row r="2" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="218"/>
@@ -2636,10 +2639,10 @@
         <v>0</v>
       </c>
       <c r="D1" s="3"/>
-      <c r="G1" s="237" t="s">
+      <c r="G1" s="250" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="238"/>
+      <c r="H1" s="251"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="4"/>
@@ -3017,7 +3020,7 @@
   <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3038,8 +3041,8 @@
     <row r="1" spans="1:22" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="74"/>
       <c r="D1" s="75"/>
-      <c r="G1" s="237"/>
-      <c r="H1" s="237"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="250"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -3100,34 +3103,34 @@
     <row r="5" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="79"/>
-      <c r="C5" s="242"/>
-      <c r="D5" s="242"/>
-      <c r="E5" s="243"/>
-      <c r="F5" s="243"/>
-      <c r="G5" s="244"/>
-      <c r="H5" s="245"/>
-      <c r="I5" s="243"/>
+      <c r="C5" s="236"/>
+      <c r="D5" s="236"/>
+      <c r="E5" s="237"/>
+      <c r="F5" s="237"/>
+      <c r="G5" s="238"/>
+      <c r="H5" s="239"/>
+      <c r="I5" s="237"/>
       <c r="J5" s="37"/>
       <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:22" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38"/>
-      <c r="B6" s="241">
+      <c r="B6" s="235">
         <v>2</v>
       </c>
-      <c r="C6" s="247" t="s">
+      <c r="C6" s="241" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="248">
+      <c r="D6" s="242">
         <f>SUM(D7:D11)/60</f>
         <v>3.5</v>
       </c>
-      <c r="E6" s="136">
+      <c r="E6" s="253">
         <f>SUM(E7:E11)/60</f>
         <v>3</v>
       </c>
       <c r="F6" s="136"/>
-      <c r="G6" s="249"/>
+      <c r="G6" s="243"/>
       <c r="H6" s="139"/>
       <c r="I6" s="141"/>
       <c r="J6" s="47"/>
@@ -3149,7 +3152,7 @@
       <c r="G7" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="246">
+      <c r="H7" s="240">
         <v>45610</v>
       </c>
       <c r="I7" s="87" t="s">
@@ -3270,7 +3273,7 @@
         <f>SUM(D13:D17)/60</f>
         <v>14</v>
       </c>
-      <c r="E12" s="239">
+      <c r="E12" s="252">
         <f>SUM(E13:E17)/60</f>
         <v>1</v>
       </c>
@@ -3294,7 +3297,7 @@
         <v>60</v>
       </c>
       <c r="F13" s="122"/>
-      <c r="G13" s="252" t="s">
+      <c r="G13" s="246" t="s">
         <v>14</v>
       </c>
       <c r="H13" s="124">
@@ -3492,8 +3495,8 @@
     <row r="1" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="74"/>
       <c r="D1" s="3"/>
-      <c r="G1" s="237"/>
-      <c r="H1" s="238"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="251"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -3640,13 +3643,13 @@
     <row r="10" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="107"/>
-      <c r="C10" s="240"/>
+      <c r="C10" s="234"/>
       <c r="D10" s="94"/>
-      <c r="E10" s="240"/>
-      <c r="F10" s="240"/>
-      <c r="G10" s="240"/>
-      <c r="H10" s="240"/>
-      <c r="I10" s="240"/>
+      <c r="E10" s="234"/>
+      <c r="F10" s="234"/>
+      <c r="G10" s="234"/>
+      <c r="H10" s="234"/>
+      <c r="I10" s="234"/>
       <c r="J10" s="104"/>
     </row>
     <row r="11" spans="1:22" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
@@ -3831,8 +3834,8 @@
     <row r="1" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="74"/>
       <c r="D1" s="3"/>
-      <c r="G1" s="237"/>
-      <c r="H1" s="238"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="251"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -3893,30 +3896,30 @@
     <row r="5" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="79"/>
-      <c r="C5" s="242"/>
-      <c r="D5" s="242"/>
-      <c r="E5" s="243"/>
-      <c r="F5" s="243"/>
-      <c r="G5" s="244"/>
-      <c r="H5" s="245"/>
-      <c r="I5" s="243"/>
+      <c r="C5" s="236"/>
+      <c r="D5" s="236"/>
+      <c r="E5" s="237"/>
+      <c r="F5" s="237"/>
+      <c r="G5" s="238"/>
+      <c r="H5" s="239"/>
+      <c r="I5" s="237"/>
       <c r="J5" s="37"/>
       <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:22" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="241">
+      <c r="B6" s="235">
         <v>6</v>
       </c>
-      <c r="C6" s="250" t="s">
+      <c r="C6" s="244" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="251">
+      <c r="D6" s="245">
         <f>SUM(D7:D9)</f>
         <v>180</v>
       </c>
       <c r="E6" s="136"/>
       <c r="F6" s="136"/>
-      <c r="G6" s="249"/>
+      <c r="G6" s="243"/>
       <c r="H6" s="139"/>
       <c r="I6" s="141"/>
       <c r="J6" s="70"/>

</xml_diff>

<commit_message>
Added all <select>'s for all fk's
</commit_message>
<xml_diff>
--- a/plans/scrum-planering.xlsx
+++ b/plans/scrum-planering.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\2024\yrkesprov\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A9448D-35CA-4BCA-AFAA-152E0A7432B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96F6265-073B-41EB-A39D-1A1E7679CAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{41C2E65D-138E-4665-8AB5-B482A8FDA31A}"/>
   </bookViews>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="108">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -449,6 +449,9 @@
   </si>
   <si>
     <t>Alla sidor som kunden kommer till är skapade</t>
+  </si>
+  <si>
+    <t>4/h 18/11/24 || Majoriteten fixad</t>
   </si>
 </sst>
 </file>
@@ -595,7 +598,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -826,11 +829,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="254">
+  <cellXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1149,9 +1165,6 @@
     <xf numFmtId="16" fontId="3" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1167,9 +1180,6 @@
     </xf>
     <xf numFmtId="14" fontId="3" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1488,6 +1498,12 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1503,12 +1519,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1705,7 +1732,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1759,7 +1786,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1813,7 +1840,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2346,8 +2373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393BB06C-F8B0-4B23-ABA1-344E8BDDC048}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2360,7 +2387,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="218"/>
+      <c r="A1" s="216"/>
       <c r="B1" s="247" t="s">
         <v>76</v>
       </c>
@@ -2370,8 +2397,8 @@
       <c r="F1" s="249"/>
     </row>
     <row r="2" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A2" s="218"/>
-      <c r="B2" s="220" t="s">
+      <c r="A2" s="216"/>
+      <c r="B2" s="218" t="s">
         <v>56</v>
       </c>
       <c r="C2" s="24" t="s">
@@ -2380,227 +2407,227 @@
       <c r="D2" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="218" t="s">
+      <c r="E2" s="216" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="219"/>
+      <c r="F2" s="217"/>
     </row>
     <row r="3" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="218"/>
-      <c r="B3" s="216" t="s">
+      <c r="A3" s="216"/>
+      <c r="B3" s="214" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="217" t="s">
+      <c r="C3" s="215" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="216"/>
-      <c r="E3" s="216" t="s">
+      <c r="D3" s="214"/>
+      <c r="E3" s="214" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="207"/>
+      <c r="F3" s="205"/>
     </row>
     <row r="4" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="197">
+      <c r="A4" s="195">
         <v>1</v>
       </c>
-      <c r="B4" s="214" t="s">
+      <c r="B4" s="212" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="209">
+      <c r="C4" s="207">
         <v>8</v>
       </c>
-      <c r="D4" s="197">
+      <c r="D4" s="195">
         <v>1</v>
       </c>
-      <c r="E4" s="208" t="s">
+      <c r="E4" s="206" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="207"/>
-      <c r="I4" s="215"/>
+      <c r="F4" s="205"/>
+      <c r="I4" s="213"/>
     </row>
     <row r="5" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="197">
+      <c r="A5" s="195">
         <v>2</v>
       </c>
-      <c r="B5" s="214" t="s">
+      <c r="B5" s="212" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="209">
+      <c r="C5" s="207">
         <v>5</v>
       </c>
-      <c r="D5" s="197">
+      <c r="D5" s="195">
         <v>2</v>
       </c>
-      <c r="E5" s="208" t="s">
+      <c r="E5" s="206" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="207"/>
+      <c r="F5" s="205"/>
     </row>
     <row r="6" spans="1:9" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="197">
+      <c r="A6" s="195">
+        <v>4</v>
+      </c>
+      <c r="B6" s="208" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="207">
+        <v>14</v>
+      </c>
+      <c r="D6" s="195">
+        <v>4</v>
+      </c>
+      <c r="E6" s="211" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="205"/>
+    </row>
+    <row r="7" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="195">
         <v>3</v>
       </c>
-      <c r="B6" s="210" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" s="209">
-        <v>14</v>
-      </c>
-      <c r="D6" s="197">
+      <c r="B7" s="209" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="207">
+        <v>7</v>
+      </c>
+      <c r="D7" s="195">
         <v>3</v>
       </c>
-      <c r="E6" s="213" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="207"/>
-    </row>
-    <row r="7" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="197">
-        <v>4</v>
-      </c>
-      <c r="B7" s="211" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="209">
-        <v>7</v>
-      </c>
-      <c r="D7" s="197">
-        <v>4</v>
-      </c>
-      <c r="E7" s="212" t="s">
+      <c r="E7" s="210" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="207"/>
+      <c r="F7" s="205"/>
     </row>
     <row r="8" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="197">
+      <c r="A8" s="195">
         <v>5</v>
       </c>
-      <c r="B8" s="211" t="s">
+      <c r="B8" s="209" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="209">
+      <c r="C8" s="207">
         <v>6</v>
       </c>
-      <c r="D8" s="197">
+      <c r="D8" s="195">
         <v>8</v>
       </c>
-      <c r="E8" s="208" t="s">
+      <c r="E8" s="206" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="207"/>
+      <c r="F8" s="205"/>
     </row>
     <row r="9" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="197">
+      <c r="A9" s="195">
         <v>6</v>
       </c>
-      <c r="B9" s="211" t="s">
+      <c r="B9" s="209" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="73">
         <v>2</v>
       </c>
-      <c r="D9" s="197">
+      <c r="D9" s="195">
         <v>5</v>
       </c>
-      <c r="E9" s="208" t="s">
+      <c r="E9" s="206" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="207"/>
+      <c r="F9" s="205"/>
     </row>
     <row r="10" spans="1:9" ht="57.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="197">
+      <c r="A10" s="195">
         <v>7</v>
       </c>
-      <c r="B10" s="210" t="s">
+      <c r="B10" s="208" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="209">
+      <c r="C10" s="207">
         <v>2</v>
       </c>
-      <c r="D10" s="197">
+      <c r="D10" s="195">
         <v>7</v>
       </c>
-      <c r="E10" s="208" t="s">
+      <c r="E10" s="206" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="207"/>
+      <c r="F10" s="205"/>
     </row>
     <row r="11" spans="1:9" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="197">
+      <c r="A11" s="195">
         <v>8</v>
       </c>
-      <c r="B11" s="208" t="s">
+      <c r="B11" s="206" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="209">
+      <c r="C11" s="207">
         <v>3</v>
       </c>
-      <c r="D11" s="197">
+      <c r="D11" s="195">
         <v>6</v>
       </c>
-      <c r="E11" s="208" t="s">
+      <c r="E11" s="206" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="207"/>
+      <c r="F11" s="205"/>
     </row>
     <row r="12" spans="1:9" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="197">
+      <c r="A12" s="195">
         <v>9</v>
       </c>
-      <c r="B12" s="210" t="s">
+      <c r="B12" s="208" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="209">
+      <c r="C12" s="207">
         <v>3</v>
       </c>
-      <c r="D12" s="197">
+      <c r="D12" s="195">
         <v>9</v>
       </c>
-      <c r="E12" s="208" t="s">
+      <c r="E12" s="206" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="207"/>
+      <c r="F12" s="205"/>
     </row>
     <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="202"/>
-      <c r="B13" s="206"/>
-      <c r="C13" s="199"/>
-      <c r="D13" s="199"/>
-      <c r="E13" s="205"/>
-      <c r="F13" s="198"/>
+      <c r="A13" s="200"/>
+      <c r="B13" s="204"/>
+      <c r="C13" s="197"/>
+      <c r="D13" s="197"/>
+      <c r="E13" s="203"/>
+      <c r="F13" s="196"/>
     </row>
     <row r="14" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="202"/>
-      <c r="B14" s="205"/>
-      <c r="C14" s="205"/>
-      <c r="D14" s="205"/>
-      <c r="E14" s="205"/>
-      <c r="F14" s="198"/>
+      <c r="A14" s="200"/>
+      <c r="B14" s="203"/>
+      <c r="C14" s="203"/>
+      <c r="D14" s="203"/>
+      <c r="E14" s="203"/>
+      <c r="F14" s="196"/>
     </row>
     <row r="15" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="204"/>
-      <c r="B15" s="205"/>
-      <c r="C15" s="204"/>
-      <c r="D15" s="204"/>
-      <c r="E15" s="203"/>
-      <c r="F15" s="198"/>
+      <c r="A15" s="202"/>
+      <c r="B15" s="203"/>
+      <c r="C15" s="202"/>
+      <c r="D15" s="202"/>
+      <c r="E15" s="201"/>
+      <c r="F15" s="196"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="202"/>
-      <c r="B16" s="201" t="s">
+      <c r="A16" s="200"/>
+      <c r="B16" s="199" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="200">
+      <c r="C16" s="198">
         <f>SUM(C4:C15)</f>
         <v>50</v>
       </c>
-      <c r="D16" s="199"/>
-      <c r="E16" s="199">
+      <c r="D16" s="197"/>
+      <c r="E16" s="197">
         <f>C16*60</f>
         <v>3000</v>
       </c>
-      <c r="F16" s="198"/>
+      <c r="F16" s="196"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2727,7 +2754,7 @@
         <f>SUM(D7:D13) / 60</f>
         <v>7.75</v>
       </c>
-      <c r="E6" s="232">
+      <c r="E6" s="230">
         <f>SUM(E7:E13)/60</f>
         <v>13.25</v>
       </c>
@@ -2757,7 +2784,7 @@
       <c r="H7" s="54">
         <v>45604</v>
       </c>
-      <c r="I7" s="221" t="s">
+      <c r="I7" s="219" t="s">
         <v>64</v>
       </c>
       <c r="J7" s="56"/>
@@ -2782,7 +2809,7 @@
       <c r="H8" s="54">
         <v>45608</v>
       </c>
-      <c r="I8" s="221" t="s">
+      <c r="I8" s="219" t="s">
         <v>65</v>
       </c>
       <c r="J8" s="56"/>
@@ -2809,7 +2836,7 @@
       <c r="H9" s="54">
         <v>45607</v>
       </c>
-      <c r="I9" s="221" t="s">
+      <c r="I9" s="219" t="s">
         <v>66</v>
       </c>
       <c r="J9" s="56"/>
@@ -2836,7 +2863,7 @@
       <c r="H10" s="54">
         <v>45607</v>
       </c>
-      <c r="I10" s="221" t="s">
+      <c r="I10" s="219" t="s">
         <v>67</v>
       </c>
       <c r="J10" s="56"/>
@@ -2861,10 +2888,10 @@
       <c r="H11" s="54">
         <v>45609</v>
       </c>
-      <c r="I11" s="221" t="s">
+      <c r="I11" s="219" t="s">
         <v>68</v>
       </c>
-      <c r="J11" s="231"/>
+      <c r="J11" s="229"/>
       <c r="K11" s="62"/>
     </row>
     <row r="12" spans="1:22" ht="61.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2886,7 +2913,7 @@
       <c r="H12" s="54">
         <v>45610</v>
       </c>
-      <c r="I12" s="221" t="s">
+      <c r="I12" s="219" t="s">
         <v>63</v>
       </c>
       <c r="J12" s="56"/>
@@ -2911,7 +2938,7 @@
       <c r="H13" s="54">
         <v>45607</v>
       </c>
-      <c r="I13" s="221" t="s">
+      <c r="I13" s="219" t="s">
         <v>69</v>
       </c>
       <c r="J13" s="56"/>
@@ -3020,7 +3047,7 @@
   <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3103,36 +3130,36 @@
     <row r="5" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="79"/>
-      <c r="C5" s="236"/>
-      <c r="D5" s="236"/>
-      <c r="E5" s="237"/>
-      <c r="F5" s="237"/>
-      <c r="G5" s="238"/>
-      <c r="H5" s="239"/>
-      <c r="I5" s="237"/>
+      <c r="C5" s="234"/>
+      <c r="D5" s="234"/>
+      <c r="E5" s="235"/>
+      <c r="F5" s="235"/>
+      <c r="G5" s="236"/>
+      <c r="H5" s="237"/>
+      <c r="I5" s="235"/>
       <c r="J5" s="37"/>
       <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:22" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38"/>
-      <c r="B6" s="235">
+      <c r="B6" s="233">
         <v>2</v>
       </c>
-      <c r="C6" s="241" t="s">
+      <c r="C6" s="239" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="242">
+      <c r="D6" s="240">
         <f>SUM(D7:D11)/60</f>
         <v>3.5</v>
       </c>
-      <c r="E6" s="253">
+      <c r="E6" s="246">
         <f>SUM(E7:E11)/60</f>
         <v>3</v>
       </c>
-      <c r="F6" s="136"/>
-      <c r="G6" s="243"/>
-      <c r="H6" s="139"/>
-      <c r="I6" s="141"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="241"/>
+      <c r="H6" s="137"/>
+      <c r="I6" s="139"/>
       <c r="J6" s="47"/>
       <c r="K6" s="7"/>
     </row>
@@ -3152,7 +3179,7 @@
       <c r="G7" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="240">
+      <c r="H7" s="238">
         <v>45610</v>
       </c>
       <c r="I7" s="87" t="s">
@@ -3230,7 +3257,7 @@
       <c r="H10" s="97">
         <v>45611</v>
       </c>
-      <c r="I10" s="194" t="s">
+      <c r="I10" s="192" t="s">
         <v>73</v>
       </c>
       <c r="J10" s="104"/>
@@ -3255,7 +3282,7 @@
       <c r="H11" s="54">
         <v>45610</v>
       </c>
-      <c r="I11" s="194" t="s">
+      <c r="I11" s="192" t="s">
         <v>74</v>
       </c>
       <c r="J11" s="104"/>
@@ -3267,146 +3294,127 @@
         <v>3</v>
       </c>
       <c r="C12" s="114" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="D12" s="114">
-        <f>SUM(D13:D17)/60</f>
-        <v>14</v>
-      </c>
-      <c r="E12" s="252">
-        <f>SUM(E13:E17)/60</f>
-        <v>1</v>
-      </c>
+        <f>SUM(D13:D15)/60</f>
+        <v>7</v>
+      </c>
+      <c r="E12" s="115"/>
       <c r="F12" s="115"/>
       <c r="G12" s="116"/>
-      <c r="H12" s="117"/>
-      <c r="I12" s="118"/>
-      <c r="J12" s="119"/>
+      <c r="H12" s="150"/>
+      <c r="I12" s="151"/>
+      <c r="J12" s="152"/>
       <c r="K12" s="17"/>
     </row>
-    <row r="13" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="104"/>
-      <c r="C13" s="215" t="s">
-        <v>105</v>
-      </c>
-      <c r="D13" s="109">
+      <c r="C13" s="119" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="120">
         <v>120</v>
       </c>
-      <c r="E13" s="122">
-        <v>60</v>
-      </c>
-      <c r="F13" s="122"/>
-      <c r="G13" s="246" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="124">
-        <v>45611</v>
-      </c>
-      <c r="I13" s="215" t="s">
-        <v>106</v>
-      </c>
-      <c r="J13" s="104"/>
+      <c r="E13" s="121"/>
+      <c r="F13" s="121"/>
+      <c r="G13" s="122"/>
+      <c r="H13" s="107"/>
+      <c r="I13" s="153" t="s">
+        <v>85</v>
+      </c>
+      <c r="J13" s="104" t="s">
+        <v>107</v>
+      </c>
       <c r="K13" s="17"/>
     </row>
-    <row r="14" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="104"/>
-      <c r="C14" s="120" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" s="121">
-        <v>240</v>
-      </c>
-      <c r="E14" s="122"/>
-      <c r="F14" s="122"/>
-      <c r="G14" s="123"/>
-      <c r="H14" s="124"/>
-      <c r="I14" s="125" t="s">
-        <v>80</v>
+      <c r="C14" s="119" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="120">
+        <v>120</v>
+      </c>
+      <c r="E14" s="121"/>
+      <c r="F14" s="121"/>
+      <c r="G14" s="122"/>
+      <c r="H14" s="107"/>
+      <c r="I14" s="153" t="s">
+        <v>88</v>
       </c>
       <c r="J14" s="104"/>
       <c r="K14" s="17"/>
     </row>
-    <row r="15" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="104"/>
-      <c r="C15" s="120" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="121">
+      <c r="C15" s="154" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="120">
         <v>180</v>
       </c>
-      <c r="E15" s="73"/>
-      <c r="F15" s="122"/>
-      <c r="G15" s="123"/>
-      <c r="H15" s="124"/>
-      <c r="I15" s="125" t="s">
-        <v>79</v>
-      </c>
-      <c r="J15" s="112"/>
+      <c r="E15" s="121"/>
+      <c r="F15" s="121"/>
+      <c r="G15" s="107"/>
+      <c r="H15" s="107"/>
+      <c r="I15" s="153" t="s">
+        <v>89</v>
+      </c>
+      <c r="J15" s="104"/>
       <c r="K15" s="17"/>
     </row>
-    <row r="16" spans="1:22" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
-      <c r="B16" s="104"/>
-      <c r="C16" s="102" t="s">
-        <v>81</v>
-      </c>
-      <c r="D16" s="102">
-        <v>180</v>
-      </c>
-      <c r="E16" s="103"/>
-      <c r="F16" s="104"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="126"/>
-      <c r="I16" s="194" t="s">
-        <v>82</v>
-      </c>
+      <c r="B16" s="232"/>
+      <c r="C16" s="232"/>
+      <c r="D16" s="232"/>
+      <c r="E16" s="232"/>
+      <c r="F16" s="232"/>
+      <c r="G16" s="232"/>
+      <c r="H16" s="232"/>
+      <c r="I16" s="232"/>
       <c r="J16" s="104"/>
       <c r="K16" s="17"/>
     </row>
     <row r="17" spans="1:11" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
-      <c r="B17" s="107"/>
-      <c r="C17" s="108" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="109">
-        <v>120</v>
-      </c>
-      <c r="E17" s="110"/>
-      <c r="F17" s="107"/>
-      <c r="G17" s="111"/>
-      <c r="H17" s="97"/>
-      <c r="I17" s="112" t="s">
-        <v>75</v>
-      </c>
+      <c r="B17" s="232"/>
+      <c r="C17" s="232"/>
+      <c r="D17" s="232"/>
+      <c r="E17" s="232"/>
+      <c r="F17" s="232"/>
+      <c r="G17" s="232"/>
+      <c r="H17" s="232"/>
+      <c r="I17" s="232"/>
       <c r="J17" s="112"/>
       <c r="K17" s="7"/>
     </row>
     <row r="18" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38"/>
-      <c r="B18" s="128"/>
-      <c r="C18" s="129" t="s">
+      <c r="B18" s="126"/>
+      <c r="C18" s="252" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="130">
-        <f>SUM(D6+D12)</f>
+      <c r="D18" s="253">
+        <f>SUM(D6+'Sprint 3 xx.xx - xx.xx'!D6)</f>
         <v>17.5</v>
       </c>
-      <c r="E18" s="71">
-        <f>SUM((E6+E12))</f>
+      <c r="E18" s="254">
+        <f>SUM((E6+'Sprint 3 xx.xx - xx.xx'!E6))</f>
         <v>4</v>
       </c>
-      <c r="F18" s="66"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
+      <c r="F18" s="255"/>
+      <c r="G18" s="126"/>
+      <c r="H18" s="126"/>
+      <c r="I18" s="126"/>
       <c r="J18" s="70"/>
     </row>
     <row r="19" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="131"/>
+      <c r="B19" s="129"/>
       <c r="C19" s="80" t="s">
         <v>24</v>
       </c>
@@ -3414,49 +3422,49 @@
         <f>SUM(D20+D18)</f>
         <v>20</v>
       </c>
-      <c r="E19" s="132"/>
-      <c r="F19" s="133"/>
+      <c r="E19" s="130"/>
+      <c r="F19" s="131"/>
       <c r="G19" s="45"/>
       <c r="H19" s="45"/>
-      <c r="I19" s="134"/>
+      <c r="I19" s="132"/>
       <c r="J19" s="72"/>
     </row>
     <row r="20" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="135"/>
-      <c r="C20" s="136" t="s">
+      <c r="B20" s="133"/>
+      <c r="C20" s="134" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="233">
+      <c r="D20" s="231">
         <v>2.5</v>
       </c>
-      <c r="E20" s="137"/>
-      <c r="F20" s="138"/>
-      <c r="G20" s="139"/>
-      <c r="H20" s="139"/>
-      <c r="I20" s="140"/>
-      <c r="J20" s="141"/>
+      <c r="E20" s="135"/>
+      <c r="F20" s="136"/>
+      <c r="G20" s="137"/>
+      <c r="H20" s="137"/>
+      <c r="I20" s="138"/>
+      <c r="J20" s="139"/>
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="142"/>
-      <c r="C21" s="143"/>
-      <c r="D21" s="143"/>
-      <c r="E21" s="144"/>
-      <c r="F21" s="145"/>
-      <c r="G21" s="146"/>
-      <c r="H21" s="146"/>
-      <c r="I21" s="147"/>
-      <c r="J21" s="148"/>
+      <c r="B21" s="140"/>
+      <c r="C21" s="141"/>
+      <c r="D21" s="141"/>
+      <c r="E21" s="142"/>
+      <c r="F21" s="143"/>
+      <c r="G21" s="144"/>
+      <c r="H21" s="144"/>
+      <c r="I21" s="145"/>
+      <c r="J21" s="146"/>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="149"/>
-      <c r="C22" s="143"/>
-      <c r="D22" s="143"/>
-      <c r="E22" s="144"/>
-      <c r="F22" s="145"/>
-      <c r="G22" s="146"/>
-      <c r="H22" s="146"/>
-      <c r="I22" s="147"/>
-      <c r="J22" s="148"/>
+      <c r="B22" s="147"/>
+      <c r="C22" s="141"/>
+      <c r="D22" s="141"/>
+      <c r="E22" s="142"/>
+      <c r="F22" s="143"/>
+      <c r="G22" s="144"/>
+      <c r="H22" s="144"/>
+      <c r="I22" s="145"/>
+      <c r="J22" s="146"/>
     </row>
     <row r="31" spans="1:11" ht="13.2" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -3471,10 +3479,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C94DF7-B35F-4481-A77A-5670F6E3A59A}">
-  <dimension ref="A1:V18"/>
+  <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3521,7 +3529,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="78"/>
       <c r="J3" s="16"/>
-      <c r="K3" s="150"/>
+      <c r="K3" s="148"/>
     </row>
     <row r="4" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
@@ -3537,7 +3545,7 @@
       <c r="E4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="151" t="s">
+      <c r="F4" s="149" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="24" t="s">
@@ -3564,7 +3572,7 @@
       <c r="G5" s="34"/>
       <c r="H5" s="35"/>
       <c r="I5" s="32"/>
-      <c r="J5" s="37"/>
+      <c r="J5" s="258"/>
       <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:22" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -3573,209 +3581,226 @@
         <v>4</v>
       </c>
       <c r="C6" s="114" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="D6" s="114">
-        <f>SUM(D7:D9)/60</f>
-        <v>7</v>
-      </c>
-      <c r="E6" s="115"/>
+        <f>SUM(D7:D11)/60</f>
+        <v>14</v>
+      </c>
+      <c r="E6" s="245">
+        <f>SUM(E7:E11)/60</f>
+        <v>1</v>
+      </c>
       <c r="F6" s="115"/>
       <c r="G6" s="116"/>
-      <c r="H6" s="152"/>
-      <c r="I6" s="153"/>
-      <c r="J6" s="154"/>
-    </row>
-    <row r="7" spans="1:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="H6" s="117"/>
+      <c r="I6" s="256"/>
+      <c r="J6" s="232"/>
+    </row>
+    <row r="7" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="104"/>
-      <c r="C7" s="120" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="121">
+      <c r="C7" s="213" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="109">
         <v>120</v>
       </c>
-      <c r="E7" s="122"/>
-      <c r="F7" s="122"/>
-      <c r="G7" s="123"/>
-      <c r="H7" s="107"/>
-      <c r="I7" s="155" t="s">
-        <v>85</v>
-      </c>
-      <c r="J7" s="104"/>
+      <c r="E7" s="121">
+        <v>60</v>
+      </c>
+      <c r="F7" s="121"/>
+      <c r="G7" s="244" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="123">
+        <v>45611</v>
+      </c>
+      <c r="I7" s="213" t="s">
+        <v>106</v>
+      </c>
+      <c r="J7" s="232"/>
     </row>
     <row r="8" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="104"/>
-      <c r="C8" s="120" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="121">
-        <v>120</v>
-      </c>
-      <c r="E8" s="122"/>
-      <c r="F8" s="122"/>
-      <c r="G8" s="123"/>
-      <c r="H8" s="107"/>
-      <c r="I8" s="155" t="s">
-        <v>88</v>
-      </c>
-      <c r="J8" s="104"/>
-    </row>
-    <row r="9" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="C8" s="119" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="120">
+        <v>240</v>
+      </c>
+      <c r="E8" s="121"/>
+      <c r="F8" s="121"/>
+      <c r="G8" s="122"/>
+      <c r="H8" s="123"/>
+      <c r="I8" s="257" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" s="232"/>
+    </row>
+    <row r="9" spans="1:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="104"/>
-      <c r="C9" s="156" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" s="121">
+      <c r="C9" s="119" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="120">
         <v>180</v>
       </c>
-      <c r="E9" s="122"/>
-      <c r="F9" s="122"/>
-      <c r="G9" s="107"/>
-      <c r="H9" s="107"/>
-      <c r="I9" s="155" t="s">
-        <v>89</v>
-      </c>
-      <c r="J9" s="104"/>
-    </row>
-    <row r="10" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="E9" s="73"/>
+      <c r="F9" s="121"/>
+      <c r="G9" s="122"/>
+      <c r="H9" s="123"/>
+      <c r="I9" s="257" t="s">
+        <v>79</v>
+      </c>
+      <c r="J9" s="232"/>
+    </row>
+    <row r="10" spans="1:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
-      <c r="B10" s="107"/>
-      <c r="C10" s="234"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="234"/>
-      <c r="F10" s="234"/>
-      <c r="G10" s="234"/>
-      <c r="H10" s="234"/>
-      <c r="I10" s="234"/>
+      <c r="B10" s="104"/>
+      <c r="C10" s="102" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="102">
+        <v>180</v>
+      </c>
+      <c r="E10" s="103"/>
+      <c r="F10" s="104"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="124"/>
+      <c r="I10" s="192" t="s">
+        <v>82</v>
+      </c>
       <c r="J10" s="104"/>
     </row>
-    <row r="11" spans="1:22" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
-      <c r="B11" s="113">
+      <c r="B11" s="107"/>
+      <c r="C11" s="108" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="109">
+        <v>120</v>
+      </c>
+      <c r="E11" s="110"/>
+      <c r="F11" s="107"/>
+      <c r="G11" s="111"/>
+      <c r="H11" s="97"/>
+      <c r="I11" s="112" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" s="104"/>
+    </row>
+    <row r="12" spans="1:22" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="113">
         <v>5</v>
       </c>
-      <c r="C11" s="114" t="s">
+      <c r="C12" s="114" t="s">
         <v>86</v>
       </c>
-      <c r="D11" s="229">
-        <f>SUM(D12:D15)/60</f>
+      <c r="D12" s="227">
+        <f>SUM(D13:D16)/60</f>
         <v>6.5</v>
       </c>
-      <c r="E11" s="115"/>
-      <c r="F11" s="115"/>
-      <c r="G11" s="157"/>
-      <c r="H11" s="157"/>
-      <c r="I11" s="153"/>
-      <c r="J11" s="119"/>
-    </row>
-    <row r="12" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="104"/>
-      <c r="C12" s="120" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="227">
-        <v>150</v>
-      </c>
-      <c r="E12" s="122"/>
-      <c r="F12" s="122"/>
-      <c r="G12" s="123"/>
-      <c r="H12" s="124"/>
-      <c r="I12" s="121" t="s">
-        <v>98</v>
-      </c>
-      <c r="J12" s="112"/>
-      <c r="K12" s="166"/>
+      <c r="E12" s="115"/>
+      <c r="F12" s="115"/>
+      <c r="G12" s="155"/>
+      <c r="H12" s="155"/>
+      <c r="I12" s="151"/>
+      <c r="J12" s="118"/>
     </row>
     <row r="13" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
-      <c r="B13" s="158"/>
-      <c r="C13" s="159" t="s">
+      <c r="B13" s="104"/>
+      <c r="C13" s="119" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="225">
+        <v>150</v>
+      </c>
+      <c r="E13" s="121"/>
+      <c r="F13" s="121"/>
+      <c r="G13" s="122"/>
+      <c r="H13" s="123"/>
+      <c r="I13" s="120" t="s">
+        <v>98</v>
+      </c>
+      <c r="J13" s="112"/>
+      <c r="K13" s="164"/>
+    </row>
+    <row r="14" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="156"/>
+      <c r="C14" s="157" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="160">
+      <c r="D14" s="158">
         <v>120</v>
       </c>
-      <c r="E13" s="161"/>
-      <c r="F13" s="161"/>
-      <c r="G13" s="162"/>
-      <c r="H13" s="163"/>
-      <c r="I13" s="164" t="s">
+      <c r="E14" s="159"/>
+      <c r="F14" s="159"/>
+      <c r="G14" s="160"/>
+      <c r="H14" s="161"/>
+      <c r="I14" s="162" t="s">
         <v>92</v>
       </c>
-      <c r="J13" s="165"/>
-      <c r="K13" s="226"/>
-    </row>
-    <row r="14" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="167"/>
-      <c r="C14" s="222" t="s">
+      <c r="J14" s="163"/>
+      <c r="K14" s="224"/>
+    </row>
+    <row r="15" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="165"/>
+      <c r="C15" s="220" t="s">
         <v>93</v>
       </c>
-      <c r="D14" s="228">
+      <c r="D15" s="226">
         <v>60</v>
       </c>
-      <c r="E14" s="168"/>
-      <c r="F14" s="168"/>
-      <c r="G14" s="169"/>
-      <c r="H14" s="170"/>
-      <c r="I14" s="223" t="s">
+      <c r="E15" s="166"/>
+      <c r="F15" s="166"/>
+      <c r="G15" s="167"/>
+      <c r="H15" s="168"/>
+      <c r="I15" s="221" t="s">
         <v>94</v>
       </c>
-      <c r="J14" s="171"/>
-      <c r="K14" s="17"/>
-    </row>
-    <row r="15" spans="1:22" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="107"/>
-      <c r="C15" s="224" t="s">
+      <c r="J15" s="169"/>
+      <c r="K15" s="17"/>
+    </row>
+    <row r="16" spans="1:22" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="107"/>
+      <c r="C16" s="222" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="127">
+      <c r="D16" s="125">
         <v>60</v>
       </c>
-      <c r="E15" s="107"/>
-      <c r="F15" s="107"/>
-      <c r="G15" s="103"/>
-      <c r="H15" s="104"/>
-      <c r="I15" s="225" t="s">
+      <c r="E16" s="107"/>
+      <c r="F16" s="107"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="104"/>
+      <c r="I16" s="223" t="s">
         <v>96</v>
       </c>
-      <c r="J15" s="112"/>
-      <c r="K15" s="7"/>
-    </row>
-    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="64"/>
-      <c r="C16" s="129" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="65">
-        <f>SUM(D6+D11)</f>
-        <v>13.5</v>
-      </c>
-      <c r="E16" s="71">
-        <f>SUM((E12+E7)/60)</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="67"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="69"/>
-      <c r="J16" s="72"/>
+      <c r="J16" s="112"/>
+      <c r="K16" s="7"/>
     </row>
     <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="64"/>
-      <c r="C17" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="65">
-        <f>SUM(D16+D18)</f>
-        <v>15</v>
-      </c>
-      <c r="E17" s="65"/>
+      <c r="C17" s="127" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="128">
+        <f>SUM('Sprint 2 xx.xx - xx.xx'!D12+D12)</f>
+        <v>13.5</v>
+      </c>
+      <c r="E17" s="71">
+        <f>SUM((E13+'Sprint 2 xx.xx - xx.xx'!E13)/60)</f>
+        <v>0</v>
+      </c>
       <c r="F17" s="67"/>
       <c r="G17" s="68"/>
       <c r="H17" s="68"/>
@@ -3785,17 +3810,33 @@
     <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="64"/>
       <c r="C18" s="65" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="65">
-        <v>1.5</v>
+        <f>SUM(D17+D19)</f>
+        <v>15</v>
       </c>
       <c r="E18" s="65"/>
       <c r="F18" s="67"/>
       <c r="G18" s="68"/>
       <c r="H18" s="68"/>
       <c r="I18" s="69"/>
-      <c r="J18" s="47"/>
+      <c r="J18" s="72"/>
+    </row>
+    <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="64"/>
+      <c r="C19" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="65">
+        <v>1.5</v>
+      </c>
+      <c r="E19" s="65"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3860,7 +3901,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="78"/>
       <c r="J3" s="16"/>
-      <c r="K3" s="150"/>
+      <c r="K3" s="148"/>
     </row>
     <row r="4" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
@@ -3896,37 +3937,37 @@
     <row r="5" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="79"/>
-      <c r="C5" s="236"/>
-      <c r="D5" s="236"/>
-      <c r="E5" s="237"/>
-      <c r="F5" s="237"/>
-      <c r="G5" s="238"/>
-      <c r="H5" s="239"/>
-      <c r="I5" s="237"/>
+      <c r="C5" s="234"/>
+      <c r="D5" s="234"/>
+      <c r="E5" s="235"/>
+      <c r="F5" s="235"/>
+      <c r="G5" s="236"/>
+      <c r="H5" s="237"/>
+      <c r="I5" s="235"/>
       <c r="J5" s="37"/>
       <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:22" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="235">
+      <c r="B6" s="233">
         <v>6</v>
       </c>
-      <c r="C6" s="244" t="s">
+      <c r="C6" s="242" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="245">
+      <c r="D6" s="243">
         <f>SUM(D7:D9)</f>
         <v>180</v>
       </c>
-      <c r="E6" s="136"/>
-      <c r="F6" s="136"/>
-      <c r="G6" s="243"/>
-      <c r="H6" s="139"/>
-      <c r="I6" s="141"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="241"/>
+      <c r="H6" s="137"/>
+      <c r="I6" s="139"/>
       <c r="J6" s="70"/>
     </row>
     <row r="7" spans="1:22" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="172"/>
-      <c r="C7" s="173" t="s">
+      <c r="B7" s="170"/>
+      <c r="C7" s="171" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="84">
@@ -3934,15 +3975,15 @@
       </c>
       <c r="E7" s="85"/>
       <c r="F7" s="85"/>
-      <c r="G7" s="174"/>
-      <c r="H7" s="175"/>
-      <c r="I7" s="176" t="s">
+      <c r="G7" s="172"/>
+      <c r="H7" s="173"/>
+      <c r="I7" s="174" t="s">
         <v>36</v>
       </c>
       <c r="J7" s="99"/>
     </row>
     <row r="8" spans="1:22" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="172"/>
+      <c r="B8" s="170"/>
       <c r="C8" s="55" t="s">
         <v>37</v>
       </c>
@@ -3956,10 +3997,10 @@
       <c r="I8" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="J8" s="177"/>
+      <c r="J8" s="175"/>
     </row>
     <row r="9" spans="1:22" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="172"/>
+      <c r="B9" s="170"/>
       <c r="C9" s="55" t="s">
         <v>38</v>
       </c>
@@ -3976,24 +4017,24 @@
       <c r="J9" s="16"/>
     </row>
     <row r="10" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="178">
+      <c r="B10" s="176">
         <v>7</v>
       </c>
-      <c r="C10" s="179" t="s">
+      <c r="C10" s="177" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="180">
+      <c r="D10" s="178">
         <v>60</v>
       </c>
-      <c r="E10" s="181"/>
-      <c r="F10" s="181"/>
-      <c r="G10" s="182"/>
-      <c r="H10" s="182"/>
-      <c r="I10" s="183"/>
-      <c r="J10" s="184"/>
+      <c r="E10" s="179"/>
+      <c r="F10" s="179"/>
+      <c r="G10" s="180"/>
+      <c r="H10" s="180"/>
+      <c r="I10" s="181"/>
+      <c r="J10" s="182"/>
     </row>
     <row r="11" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="185"/>
+      <c r="B11" s="183"/>
       <c r="C11" s="55" t="s">
         <v>39</v>
       </c>
@@ -4010,59 +4051,59 @@
       <c r="J11" s="99"/>
     </row>
     <row r="12" spans="1:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="178">
+      <c r="B12" s="176">
         <v>8</v>
       </c>
-      <c r="C12" s="186" t="s">
+      <c r="C12" s="184" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="187">
+      <c r="D12" s="185">
         <v>60</v>
       </c>
-      <c r="E12" s="188"/>
-      <c r="F12" s="188"/>
-      <c r="G12" s="189"/>
-      <c r="H12" s="189"/>
-      <c r="I12" s="190"/>
-      <c r="J12" s="191"/>
+      <c r="E12" s="186"/>
+      <c r="F12" s="186"/>
+      <c r="G12" s="187"/>
+      <c r="H12" s="187"/>
+      <c r="I12" s="188"/>
+      <c r="J12" s="189"/>
     </row>
     <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="104"/>
-      <c r="C13" s="192" t="s">
+      <c r="C13" s="190" t="s">
         <v>40</v>
       </c>
       <c r="D13" s="110">
         <v>60</v>
       </c>
-      <c r="E13" s="193"/>
-      <c r="F13" s="193"/>
+      <c r="E13" s="191"/>
+      <c r="F13" s="191"/>
       <c r="G13" s="104"/>
       <c r="H13" s="104"/>
-      <c r="I13" s="230" t="s">
+      <c r="I13" s="228" t="s">
         <v>102</v>
       </c>
       <c r="J13" s="112"/>
     </row>
     <row r="14" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="157">
+      <c r="B14" s="155">
         <v>9</v>
       </c>
-      <c r="C14" s="195" t="s">
+      <c r="C14" s="193" t="s">
         <v>41</v>
       </c>
       <c r="D14" s="116">
         <v>120</v>
       </c>
-      <c r="E14" s="157"/>
-      <c r="F14" s="157"/>
-      <c r="G14" s="196"/>
-      <c r="H14" s="119"/>
-      <c r="I14" s="154"/>
-      <c r="J14" s="154"/>
+      <c r="E14" s="155"/>
+      <c r="F14" s="155"/>
+      <c r="G14" s="194"/>
+      <c r="H14" s="118"/>
+      <c r="I14" s="152"/>
+      <c r="J14" s="152"/>
     </row>
     <row r="15" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B15" s="172"/>
-      <c r="C15" s="173" t="s">
+      <c r="B15" s="170"/>
+      <c r="C15" s="171" t="s">
         <v>41</v>
       </c>
       <c r="D15" s="84">
@@ -4070,13 +4111,13 @@
       </c>
       <c r="E15" s="85"/>
       <c r="F15" s="85"/>
-      <c r="G15" s="174"/>
-      <c r="H15" s="175"/>
-      <c r="I15" s="176"/>
+      <c r="G15" s="172"/>
+      <c r="H15" s="173"/>
+      <c r="I15" s="174"/>
       <c r="J15" s="99"/>
     </row>
     <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="172"/>
+      <c r="B16" s="170"/>
       <c r="C16" s="90"/>
       <c r="D16" s="50"/>
       <c r="E16" s="51"/>
@@ -4084,11 +4125,11 @@
       <c r="G16" s="60"/>
       <c r="H16" s="20"/>
       <c r="I16" s="90"/>
-      <c r="J16" s="177"/>
+      <c r="J16" s="175"/>
     </row>
     <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="64"/>
-      <c r="C17" s="129" t="s">
+      <c r="C17" s="127" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="65">
@@ -4110,7 +4151,7 @@
       <c r="C18" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="129"/>
+      <c r="D18" s="127"/>
       <c r="E18" s="65"/>
       <c r="F18" s="67"/>
       <c r="G18" s="68"/>

</xml_diff>

<commit_message>
Book insert query added
</commit_message>
<xml_diff>
--- a/plans/scrum-planering.xlsx
+++ b/plans/scrum-planering.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\2024\yrkesprov\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96F6265-073B-41EB-A39D-1A1E7679CAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41395442-97BF-4E20-B1CC-0C9001FD7B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{41C2E65D-138E-4665-8AB5-B482A8FDA31A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{41C2E65D-138E-4665-8AB5-B482A8FDA31A}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="7" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="108">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -238,9 +238,6 @@
     <t>Säkerhetstestning</t>
   </si>
   <si>
-    <t>Prepared querys, htacces och sanitize input</t>
-  </si>
-  <si>
     <t>Funktionalitetstestning</t>
   </si>
   <si>
@@ -452,6 +449,9 @@
   </si>
   <si>
     <t>4/h 18/11/24 || Majoriteten fixad</t>
+  </si>
+  <si>
+    <t>Prepared querys, htacces, block user access, sanitize input and ?</t>
   </si>
 </sst>
 </file>
@@ -846,7 +846,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="259">
+  <cellXfs count="260">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1504,28 +1504,10 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1536,6 +1518,27 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2374,7 +2377,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2388,41 +2391,41 @@
   <sheetData>
     <row r="1" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="216"/>
-      <c r="B1" s="247" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="248"/>
-      <c r="D1" s="248"/>
-      <c r="E1" s="248"/>
-      <c r="F1" s="249"/>
+      <c r="B1" s="253" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="254"/>
+      <c r="D1" s="254"/>
+      <c r="E1" s="254"/>
+      <c r="F1" s="255"/>
     </row>
     <row r="2" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="216"/>
       <c r="B2" s="218" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" s="216" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" s="217"/>
     </row>
     <row r="3" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="216"/>
       <c r="B3" s="214" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="215" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="214"/>
       <c r="E3" s="214" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F3" s="205"/>
     </row>
@@ -2440,7 +2443,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="206" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" s="205"/>
       <c r="I4" s="213"/>
@@ -2450,7 +2453,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="212" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="207">
         <v>5</v>
@@ -2459,7 +2462,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="206" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5" s="205"/>
     </row>
@@ -2468,7 +2471,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="208" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C6" s="207">
         <v>14</v>
@@ -2477,7 +2480,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="211" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F6" s="205"/>
     </row>
@@ -2486,7 +2489,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="209" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="207">
         <v>7</v>
@@ -2495,7 +2498,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="210" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" s="205"/>
     </row>
@@ -2504,7 +2507,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="209" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="207">
         <v>6</v>
@@ -2513,7 +2516,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="206" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F8" s="205"/>
     </row>
@@ -2531,7 +2534,7 @@
         <v>5</v>
       </c>
       <c r="E9" s="206" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" s="205"/>
     </row>
@@ -2540,16 +2543,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="208" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="207">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="195">
         <v>7</v>
       </c>
       <c r="E10" s="206" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" s="205"/>
     </row>
@@ -2558,16 +2561,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="206" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="207">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11" s="195">
         <v>6</v>
       </c>
       <c r="E11" s="206" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F11" s="205"/>
     </row>
@@ -2576,7 +2579,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="208" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="207">
         <v>3</v>
@@ -2585,7 +2588,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="206" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F12" s="205"/>
     </row>
@@ -2616,16 +2619,16 @@
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="200"/>
       <c r="B16" s="199" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="198">
         <f>SUM(C4:C15)</f>
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D16" s="197"/>
       <c r="E16" s="197">
         <f>C16*60</f>
-        <v>3000</v>
+        <v>2820</v>
       </c>
       <c r="F16" s="196"/>
     </row>
@@ -2642,7 +2645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{890CFAFE-5C64-4A48-A718-920F5088B08F}">
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -2666,10 +2669,10 @@
         <v>0</v>
       </c>
       <c r="D1" s="3"/>
-      <c r="G1" s="250" t="s">
+      <c r="G1" s="256" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="251"/>
+      <c r="H1" s="257"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="4"/>
@@ -2785,7 +2788,7 @@
         <v>45604</v>
       </c>
       <c r="I7" s="219" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J7" s="56"/>
       <c r="K7" s="6"/>
@@ -2810,7 +2813,7 @@
         <v>45608</v>
       </c>
       <c r="I8" s="219" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J8" s="56"/>
       <c r="K8" s="57" t="s">
@@ -2837,7 +2840,7 @@
         <v>45607</v>
       </c>
       <c r="I9" s="219" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J9" s="56"/>
       <c r="K9" s="59" t="s">
@@ -2864,7 +2867,7 @@
         <v>45607</v>
       </c>
       <c r="I10" s="219" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J10" s="56"/>
       <c r="K10" s="61"/>
@@ -2889,7 +2892,7 @@
         <v>45609</v>
       </c>
       <c r="I11" s="219" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J11" s="229"/>
       <c r="K11" s="62"/>
@@ -2914,7 +2917,7 @@
         <v>45610</v>
       </c>
       <c r="I12" s="219" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J12" s="56"/>
       <c r="K12" s="62"/>
@@ -2939,7 +2942,7 @@
         <v>45607</v>
       </c>
       <c r="I13" s="219" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J13" s="56"/>
       <c r="K13" s="62"/>
@@ -3046,8 +3049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF3BD90-0203-44B4-AE4B-CE188AD45574}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3068,8 +3071,8 @@
     <row r="1" spans="1:22" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="74"/>
       <c r="D1" s="75"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="250"/>
+      <c r="G1" s="256"/>
+      <c r="H1" s="256"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -3146,7 +3149,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="239" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" s="240">
         <f>SUM(D7:D11)/60</f>
@@ -3183,7 +3186,7 @@
         <v>45610</v>
       </c>
       <c r="I7" s="87" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="88"/>
@@ -3208,7 +3211,7 @@
         <v>45610</v>
       </c>
       <c r="I8" s="87" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J8" s="56"/>
       <c r="K8" s="88"/>
@@ -3233,7 +3236,7 @@
         <v>45611</v>
       </c>
       <c r="I9" s="98" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J9" s="99"/>
       <c r="K9" s="17"/>
@@ -3258,7 +3261,7 @@
         <v>45611</v>
       </c>
       <c r="I10" s="192" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J10" s="104"/>
       <c r="K10" s="17"/>
@@ -3283,7 +3286,7 @@
         <v>45610</v>
       </c>
       <c r="I11" s="192" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J11" s="104"/>
       <c r="K11" s="17"/>
@@ -3294,13 +3297,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="114" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D12" s="114">
         <f>SUM(D13:D15)/60</f>
         <v>7</v>
       </c>
-      <c r="E12" s="115"/>
+      <c r="E12" s="245">
+        <f>SUM(E13:E17)/60</f>
+        <v>7</v>
+      </c>
       <c r="F12" s="115"/>
       <c r="G12" s="116"/>
       <c r="H12" s="150"/>
@@ -3312,20 +3318,26 @@
       <c r="A13" s="7"/>
       <c r="B13" s="104"/>
       <c r="C13" s="119" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13" s="120">
         <v>120</v>
       </c>
-      <c r="E13" s="121"/>
+      <c r="E13" s="258">
+        <v>360</v>
+      </c>
       <c r="F13" s="121"/>
-      <c r="G13" s="122"/>
-      <c r="H13" s="107"/>
+      <c r="G13" s="244" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="123">
+        <v>45615</v>
+      </c>
       <c r="I13" s="153" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J13" s="104" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K13" s="17"/>
     </row>
@@ -3333,17 +3345,23 @@
       <c r="A14" s="7"/>
       <c r="B14" s="104"/>
       <c r="C14" s="119" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D14" s="120">
         <v>120</v>
       </c>
-      <c r="E14" s="121"/>
+      <c r="E14" s="258">
+        <v>60</v>
+      </c>
       <c r="F14" s="121"/>
-      <c r="G14" s="122"/>
-      <c r="H14" s="107"/>
+      <c r="G14" s="122" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="123">
+        <v>45616</v>
+      </c>
       <c r="I14" s="153" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J14" s="104"/>
       <c r="K14" s="17"/>
@@ -3352,7 +3370,7 @@
       <c r="A15" s="7"/>
       <c r="B15" s="104"/>
       <c r="C15" s="154" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D15" s="120">
         <v>180</v>
@@ -3362,7 +3380,7 @@
       <c r="G15" s="107"/>
       <c r="H15" s="107"/>
       <c r="I15" s="153" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J15" s="104"/>
       <c r="K15" s="17"/>
@@ -3396,18 +3414,18 @@
     <row r="18" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38"/>
       <c r="B18" s="126"/>
-      <c r="C18" s="252" t="s">
+      <c r="C18" s="247" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="253">
-        <f>SUM(D6+'Sprint 3 xx.xx - xx.xx'!D6)</f>
-        <v>17.5</v>
-      </c>
-      <c r="E18" s="254">
-        <f>SUM((E6+'Sprint 3 xx.xx - xx.xx'!E6))</f>
-        <v>4</v>
-      </c>
-      <c r="F18" s="255"/>
+      <c r="D18" s="248">
+        <f>SUM(D6+D12)</f>
+        <v>10.5</v>
+      </c>
+      <c r="E18" s="259">
+        <f>SUM(E6+E12)</f>
+        <v>10</v>
+      </c>
+      <c r="F18" s="249"/>
       <c r="G18" s="126"/>
       <c r="H18" s="126"/>
       <c r="I18" s="126"/>
@@ -3420,7 +3438,7 @@
       </c>
       <c r="D19" s="42">
         <f>SUM(D20+D18)</f>
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E19" s="130"/>
       <c r="F19" s="131"/>
@@ -3482,7 +3500,7 @@
   <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3503,8 +3521,8 @@
     <row r="1" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="74"/>
       <c r="D1" s="3"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="G1" s="256"/>
+      <c r="H1" s="257"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -3572,7 +3590,7 @@
       <c r="G5" s="34"/>
       <c r="H5" s="35"/>
       <c r="I5" s="32"/>
-      <c r="J5" s="258"/>
+      <c r="J5" s="252"/>
       <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:22" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -3581,7 +3599,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="114" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" s="114">
         <f>SUM(D7:D11)/60</f>
@@ -3594,14 +3612,14 @@
       <c r="F6" s="115"/>
       <c r="G6" s="116"/>
       <c r="H6" s="117"/>
-      <c r="I6" s="256"/>
+      <c r="I6" s="250"/>
       <c r="J6" s="232"/>
     </row>
     <row r="7" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="104"/>
       <c r="C7" s="213" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7" s="109">
         <v>120</v>
@@ -3617,7 +3635,7 @@
         <v>45611</v>
       </c>
       <c r="I7" s="213" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J7" s="232"/>
     </row>
@@ -3625,7 +3643,7 @@
       <c r="A8" s="8"/>
       <c r="B8" s="104"/>
       <c r="C8" s="119" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" s="120">
         <v>240</v>
@@ -3634,8 +3652,8 @@
       <c r="F8" s="121"/>
       <c r="G8" s="122"/>
       <c r="H8" s="123"/>
-      <c r="I8" s="257" t="s">
-        <v>80</v>
+      <c r="I8" s="251" t="s">
+        <v>79</v>
       </c>
       <c r="J8" s="232"/>
     </row>
@@ -3643,7 +3661,7 @@
       <c r="A9" s="8"/>
       <c r="B9" s="104"/>
       <c r="C9" s="119" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9" s="120">
         <v>180</v>
@@ -3652,8 +3670,8 @@
       <c r="F9" s="121"/>
       <c r="G9" s="122"/>
       <c r="H9" s="123"/>
-      <c r="I9" s="257" t="s">
-        <v>79</v>
+      <c r="I9" s="251" t="s">
+        <v>78</v>
       </c>
       <c r="J9" s="232"/>
     </row>
@@ -3661,7 +3679,7 @@
       <c r="A10" s="8"/>
       <c r="B10" s="104"/>
       <c r="C10" s="102" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D10" s="102">
         <v>180</v>
@@ -3671,7 +3689,7 @@
       <c r="G10" s="105"/>
       <c r="H10" s="124"/>
       <c r="I10" s="192" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J10" s="104"/>
     </row>
@@ -3689,7 +3707,7 @@
       <c r="G11" s="111"/>
       <c r="H11" s="97"/>
       <c r="I11" s="112" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J11" s="104"/>
     </row>
@@ -3699,11 +3717,11 @@
         <v>5</v>
       </c>
       <c r="C12" s="114" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D12" s="227">
         <f>SUM(D13:D16)/60</f>
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="E12" s="115"/>
       <c r="F12" s="115"/>
@@ -3716,17 +3734,17 @@
       <c r="A13" s="8"/>
       <c r="B13" s="104"/>
       <c r="C13" s="119" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" s="225">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="E13" s="121"/>
       <c r="F13" s="121"/>
       <c r="G13" s="122"/>
       <c r="H13" s="123"/>
       <c r="I13" s="120" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J13" s="112"/>
       <c r="K13" s="164"/>
@@ -3735,7 +3753,7 @@
       <c r="A14" s="8"/>
       <c r="B14" s="156"/>
       <c r="C14" s="157" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D14" s="158">
         <v>120</v>
@@ -3745,7 +3763,7 @@
       <c r="G14" s="160"/>
       <c r="H14" s="161"/>
       <c r="I14" s="162" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J14" s="163"/>
       <c r="K14" s="224"/>
@@ -3754,7 +3772,7 @@
       <c r="A15" s="8"/>
       <c r="B15" s="165"/>
       <c r="C15" s="220" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D15" s="226">
         <v>60</v>
@@ -3764,7 +3782,7 @@
       <c r="G15" s="167"/>
       <c r="H15" s="168"/>
       <c r="I15" s="221" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J15" s="169"/>
       <c r="K15" s="17"/>
@@ -3773,7 +3791,7 @@
       <c r="A16" s="17"/>
       <c r="B16" s="107"/>
       <c r="C16" s="222" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D16" s="125">
         <v>60</v>
@@ -3783,7 +3801,7 @@
       <c r="G16" s="103"/>
       <c r="H16" s="104"/>
       <c r="I16" s="223" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J16" s="112"/>
       <c r="K16" s="7"/>
@@ -3794,12 +3812,12 @@
         <v>33</v>
       </c>
       <c r="D17" s="128">
-        <f>SUM('Sprint 2 xx.xx - xx.xx'!D12+D12)</f>
-        <v>13.5</v>
+        <f>SUM(D6+D12)</f>
+        <v>21</v>
       </c>
       <c r="E17" s="71">
         <f>SUM((E13+'Sprint 2 xx.xx - xx.xx'!E13)/60)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F17" s="67"/>
       <c r="G17" s="68"/>
@@ -3814,7 +3832,7 @@
       </c>
       <c r="D18" s="65">
         <f>SUM(D17+D19)</f>
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E18" s="65"/>
       <c r="F18" s="67"/>
@@ -3829,7 +3847,7 @@
         <v>25</v>
       </c>
       <c r="D19" s="65">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E19" s="65"/>
       <c r="F19" s="67"/>
@@ -3853,8 +3871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA02060-17A8-4F90-AA70-CE39812F4F3A}">
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3875,8 +3893,8 @@
     <row r="1" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="74"/>
       <c r="D1" s="3"/>
-      <c r="G1" s="250"/>
-      <c r="H1" s="251"/>
+      <c r="G1" s="256"/>
+      <c r="H1" s="257"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -3978,14 +3996,14 @@
       <c r="G7" s="172"/>
       <c r="H7" s="173"/>
       <c r="I7" s="174" t="s">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="J7" s="99"/>
     </row>
     <row r="8" spans="1:22" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="170"/>
       <c r="C8" s="55" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="50">
         <v>60</v>
@@ -3995,14 +4013,14 @@
       <c r="G8" s="60"/>
       <c r="H8" s="20"/>
       <c r="I8" s="55" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J8" s="175"/>
     </row>
     <row r="9" spans="1:22" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="170"/>
       <c r="C9" s="55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="50">
         <v>60</v>
@@ -4012,7 +4030,7 @@
       <c r="G9" s="60"/>
       <c r="H9" s="20"/>
       <c r="I9" s="55" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J9" s="16"/>
     </row>
@@ -4021,7 +4039,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="177" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="178">
         <v>60</v>
@@ -4036,7 +4054,7 @@
     <row r="11" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="183"/>
       <c r="C11" s="55" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="50">
         <v>60</v>
@@ -4046,7 +4064,7 @@
       <c r="G11" s="60"/>
       <c r="H11" s="20"/>
       <c r="I11" s="55" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J11" s="99"/>
     </row>
@@ -4055,7 +4073,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="184" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="185">
         <v>60</v>
@@ -4070,7 +4088,7 @@
     <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="104"/>
       <c r="C13" s="190" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="110">
         <v>60</v>
@@ -4080,7 +4098,7 @@
       <c r="G13" s="104"/>
       <c r="H13" s="104"/>
       <c r="I13" s="228" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J13" s="112"/>
     </row>
@@ -4089,7 +4107,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="193" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="116">
         <v>120</v>
@@ -4104,7 +4122,7 @@
     <row r="15" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B15" s="170"/>
       <c r="C15" s="171" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15" s="84">
         <v>120</v>

</xml_diff>

<commit_message>
Book string data can be edited
</commit_message>
<xml_diff>
--- a/plans/scrum-planering.xlsx
+++ b/plans/scrum-planering.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\2024\yrkesprov\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41395442-97BF-4E20-B1CC-0C9001FD7B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1028979C-3477-4A75-A6C1-0DE0D7E646A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{41C2E65D-138E-4665-8AB5-B482A8FDA31A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{41C2E65D-138E-4665-8AB5-B482A8FDA31A}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="7" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="109">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -452,6 +452,9 @@
   </si>
   <si>
     <t>Prepared querys, htacces, block user access, sanitize input and ?</t>
+  </si>
+  <si>
+    <t>2/h 20/11/24                                   4/h 21/11/24 || Edit funkar till vissa saker, expandera senare</t>
   </si>
 </sst>
 </file>
@@ -846,7 +849,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="260">
+  <cellXfs count="261">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1446,9 +1449,6 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1518,6 +1518,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1533,11 +1539,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1735,7 +1741,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1789,7 +1795,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1843,7 +1849,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2391,13 +2397,13 @@
   <sheetData>
     <row r="1" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="216"/>
-      <c r="B1" s="253" t="s">
+      <c r="B1" s="254" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="254"/>
-      <c r="D1" s="254"/>
-      <c r="E1" s="254"/>
-      <c r="F1" s="255"/>
+      <c r="C1" s="255"/>
+      <c r="D1" s="255"/>
+      <c r="E1" s="255"/>
+      <c r="F1" s="256"/>
     </row>
     <row r="2" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="216"/>
@@ -2669,10 +2675,10 @@
         <v>0</v>
       </c>
       <c r="D1" s="3"/>
-      <c r="G1" s="256" t="s">
+      <c r="G1" s="257" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="257"/>
+      <c r="H1" s="258"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="4"/>
@@ -2757,7 +2763,7 @@
         <f>SUM(D7:D13) / 60</f>
         <v>7.75</v>
       </c>
-      <c r="E6" s="230">
+      <c r="E6" s="229">
         <f>SUM(E7:E13)/60</f>
         <v>13.25</v>
       </c>
@@ -2894,7 +2900,7 @@
       <c r="I11" s="219" t="s">
         <v>67</v>
       </c>
-      <c r="J11" s="229"/>
+      <c r="J11" s="228"/>
       <c r="K11" s="62"/>
     </row>
     <row r="12" spans="1:22" ht="61.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3049,8 +3055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF3BD90-0203-44B4-AE4B-CE188AD45574}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3071,8 +3077,8 @@
     <row r="1" spans="1:22" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="74"/>
       <c r="D1" s="75"/>
-      <c r="G1" s="256"/>
-      <c r="H1" s="256"/>
+      <c r="G1" s="257"/>
+      <c r="H1" s="257"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -3133,34 +3139,34 @@
     <row r="5" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="79"/>
-      <c r="C5" s="234"/>
-      <c r="D5" s="234"/>
-      <c r="E5" s="235"/>
-      <c r="F5" s="235"/>
-      <c r="G5" s="236"/>
-      <c r="H5" s="237"/>
-      <c r="I5" s="235"/>
+      <c r="C5" s="233"/>
+      <c r="D5" s="233"/>
+      <c r="E5" s="234"/>
+      <c r="F5" s="234"/>
+      <c r="G5" s="235"/>
+      <c r="H5" s="236"/>
+      <c r="I5" s="234"/>
       <c r="J5" s="37"/>
       <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:22" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38"/>
-      <c r="B6" s="233">
+      <c r="B6" s="232">
         <v>2</v>
       </c>
-      <c r="C6" s="239" t="s">
+      <c r="C6" s="238" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="240">
+      <c r="D6" s="239">
         <f>SUM(D7:D11)/60</f>
         <v>3.5</v>
       </c>
-      <c r="E6" s="246">
+      <c r="E6" s="245">
         <f>SUM(E7:E11)/60</f>
         <v>3</v>
       </c>
       <c r="F6" s="134"/>
-      <c r="G6" s="241"/>
+      <c r="G6" s="240"/>
       <c r="H6" s="137"/>
       <c r="I6" s="139"/>
       <c r="J6" s="47"/>
@@ -3182,7 +3188,7 @@
       <c r="G7" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="238">
+      <c r="H7" s="237">
         <v>45610</v>
       </c>
       <c r="I7" s="87" t="s">
@@ -3303,7 +3309,7 @@
         <f>SUM(D13:D15)/60</f>
         <v>7</v>
       </c>
-      <c r="E12" s="245">
+      <c r="E12" s="244">
         <f>SUM(E13:E17)/60</f>
         <v>7</v>
       </c>
@@ -3323,11 +3329,11 @@
       <c r="D13" s="120">
         <v>120</v>
       </c>
-      <c r="E13" s="258">
+      <c r="E13" s="252">
         <v>360</v>
       </c>
       <c r="F13" s="121"/>
-      <c r="G13" s="244" t="s">
+      <c r="G13" s="243" t="s">
         <v>14</v>
       </c>
       <c r="H13" s="123">
@@ -3350,7 +3356,7 @@
       <c r="D14" s="120">
         <v>120</v>
       </c>
-      <c r="E14" s="258">
+      <c r="E14" s="252">
         <v>60</v>
       </c>
       <c r="F14" s="121"/>
@@ -3366,7 +3372,7 @@
       <c r="J14" s="104"/>
       <c r="K14" s="17"/>
     </row>
-    <row r="15" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="104"/>
       <c r="C15" s="154" t="s">
@@ -3382,50 +3388,52 @@
       <c r="I15" s="153" t="s">
         <v>88</v>
       </c>
-      <c r="J15" s="104"/>
+      <c r="J15" s="192" t="s">
+        <v>108</v>
+      </c>
       <c r="K15" s="17"/>
     </row>
     <row r="16" spans="1:22" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
-      <c r="B16" s="232"/>
-      <c r="C16" s="232"/>
-      <c r="D16" s="232"/>
-      <c r="E16" s="232"/>
-      <c r="F16" s="232"/>
-      <c r="G16" s="232"/>
-      <c r="H16" s="232"/>
-      <c r="I16" s="232"/>
+      <c r="B16" s="231"/>
+      <c r="C16" s="231"/>
+      <c r="D16" s="231"/>
+      <c r="E16" s="231"/>
+      <c r="F16" s="231"/>
+      <c r="G16" s="231"/>
+      <c r="H16" s="231"/>
+      <c r="I16" s="231"/>
       <c r="J16" s="104"/>
       <c r="K16" s="17"/>
     </row>
     <row r="17" spans="1:11" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
-      <c r="B17" s="232"/>
-      <c r="C17" s="232"/>
-      <c r="D17" s="232"/>
-      <c r="E17" s="232"/>
-      <c r="F17" s="232"/>
-      <c r="G17" s="232"/>
-      <c r="H17" s="232"/>
-      <c r="I17" s="232"/>
+      <c r="B17" s="231"/>
+      <c r="C17" s="231"/>
+      <c r="D17" s="231"/>
+      <c r="E17" s="231"/>
+      <c r="F17" s="231"/>
+      <c r="G17" s="231"/>
+      <c r="H17" s="231"/>
+      <c r="I17" s="231"/>
       <c r="J17" s="112"/>
       <c r="K17" s="7"/>
     </row>
     <row r="18" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38"/>
       <c r="B18" s="126"/>
-      <c r="C18" s="247" t="s">
+      <c r="C18" s="246" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="248">
+      <c r="D18" s="247">
         <f>SUM(D6+D12)</f>
         <v>10.5</v>
       </c>
-      <c r="E18" s="259">
+      <c r="E18" s="253">
         <f>SUM(E6+E12)</f>
         <v>10</v>
       </c>
-      <c r="F18" s="249"/>
+      <c r="F18" s="248"/>
       <c r="G18" s="126"/>
       <c r="H18" s="126"/>
       <c r="I18" s="126"/>
@@ -3452,7 +3460,7 @@
       <c r="C20" s="134" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="231">
+      <c r="D20" s="230">
         <v>2.5</v>
       </c>
       <c r="E20" s="135"/>
@@ -3497,10 +3505,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C94DF7-B35F-4481-A77A-5670F6E3A59A}">
-  <dimension ref="A1:V19"/>
+  <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3521,8 +3529,8 @@
     <row r="1" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="74"/>
       <c r="D1" s="3"/>
-      <c r="G1" s="256"/>
-      <c r="H1" s="257"/>
+      <c r="G1" s="257"/>
+      <c r="H1" s="258"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -3590,7 +3598,7 @@
       <c r="G5" s="34"/>
       <c r="H5" s="35"/>
       <c r="I5" s="32"/>
-      <c r="J5" s="252"/>
+      <c r="J5" s="251"/>
       <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:22" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -3602,18 +3610,18 @@
         <v>103</v>
       </c>
       <c r="D6" s="114">
-        <f>SUM(D7:D11)/60</f>
-        <v>14</v>
-      </c>
-      <c r="E6" s="245">
-        <f>SUM(E7:E11)/60</f>
-        <v>1</v>
+        <f>SUM(D7:D10)/60</f>
+        <v>12</v>
+      </c>
+      <c r="E6" s="244">
+        <f>SUM(E7:E13)/60</f>
+        <v>1.0333333333333334</v>
       </c>
       <c r="F6" s="115"/>
       <c r="G6" s="116"/>
       <c r="H6" s="117"/>
-      <c r="I6" s="250"/>
-      <c r="J6" s="232"/>
+      <c r="I6" s="249"/>
+      <c r="J6" s="231"/>
     </row>
     <row r="7" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
@@ -3628,7 +3636,7 @@
         <v>60</v>
       </c>
       <c r="F7" s="121"/>
-      <c r="G7" s="244" t="s">
+      <c r="G7" s="243" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="123">
@@ -3637,7 +3645,7 @@
       <c r="I7" s="213" t="s">
         <v>105</v>
       </c>
-      <c r="J7" s="232"/>
+      <c r="J7" s="231"/>
     </row>
     <row r="8" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
@@ -3652,10 +3660,10 @@
       <c r="F8" s="121"/>
       <c r="G8" s="122"/>
       <c r="H8" s="123"/>
-      <c r="I8" s="251" t="s">
+      <c r="I8" s="250" t="s">
         <v>79</v>
       </c>
-      <c r="J8" s="232"/>
+      <c r="J8" s="231"/>
     </row>
     <row r="9" spans="1:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
@@ -3670,10 +3678,10 @@
       <c r="F9" s="121"/>
       <c r="G9" s="122"/>
       <c r="H9" s="123"/>
-      <c r="I9" s="251" t="s">
+      <c r="I9" s="250" t="s">
         <v>78</v>
       </c>
-      <c r="J9" s="232"/>
+      <c r="J9" s="231"/>
     </row>
     <row r="10" spans="1:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
@@ -3694,22 +3702,16 @@
       <c r="J10" s="104"/>
     </row>
     <row r="11" spans="1:22" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="107"/>
-      <c r="C11" s="108" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="109">
-        <v>120</v>
-      </c>
-      <c r="E11" s="110"/>
-      <c r="F11" s="107"/>
-      <c r="G11" s="111"/>
-      <c r="H11" s="97"/>
-      <c r="I11" s="112" t="s">
-        <v>74</v>
-      </c>
-      <c r="J11" s="104"/>
+      <c r="A11" s="259"/>
+      <c r="B11" s="231"/>
+      <c r="C11" s="231"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="231"/>
+      <c r="F11" s="231"/>
+      <c r="G11" s="231"/>
+      <c r="H11" s="231"/>
+      <c r="I11" s="231"/>
+      <c r="J11" s="231"/>
     </row>
     <row r="12" spans="1:22" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
@@ -3719,9 +3721,9 @@
       <c r="C12" s="114" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="227">
-        <f>SUM(D13:D16)/60</f>
-        <v>7</v>
+      <c r="D12" s="260">
+        <f>SUM(D13:D17)/60</f>
+        <v>9</v>
       </c>
       <c r="E12" s="115"/>
       <c r="F12" s="115"/>
@@ -3730,138 +3732,162 @@
       <c r="I12" s="151"/>
       <c r="J12" s="118"/>
     </row>
-    <row r="13" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
-      <c r="B13" s="104"/>
-      <c r="C13" s="119" t="s">
-        <v>96</v>
-      </c>
-      <c r="D13" s="225">
-        <v>180</v>
-      </c>
-      <c r="E13" s="121"/>
-      <c r="F13" s="121"/>
-      <c r="G13" s="122"/>
-      <c r="H13" s="123"/>
-      <c r="I13" s="120" t="s">
-        <v>97</v>
-      </c>
-      <c r="J13" s="112"/>
-      <c r="K13" s="164"/>
+      <c r="B13" s="107"/>
+      <c r="C13" s="108" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="109">
+        <v>120</v>
+      </c>
+      <c r="E13" s="110">
+        <v>2</v>
+      </c>
+      <c r="F13" s="107"/>
+      <c r="G13" s="111" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="97">
+        <v>45621</v>
+      </c>
+      <c r="I13" s="225" t="s">
+        <v>74</v>
+      </c>
+      <c r="J13" s="104"/>
     </row>
     <row r="14" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
-      <c r="B14" s="156"/>
-      <c r="C14" s="157" t="s">
+      <c r="B14" s="104"/>
+      <c r="C14" s="119" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="225">
+        <v>180</v>
+      </c>
+      <c r="E14" s="121"/>
+      <c r="F14" s="121"/>
+      <c r="G14" s="122"/>
+      <c r="H14" s="123"/>
+      <c r="I14" s="120" t="s">
+        <v>97</v>
+      </c>
+      <c r="J14" s="112"/>
+      <c r="K14" s="164"/>
+    </row>
+    <row r="15" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="156"/>
+      <c r="C15" s="157" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="158">
+      <c r="D15" s="158">
         <v>120</v>
       </c>
-      <c r="E14" s="159"/>
-      <c r="F14" s="159"/>
-      <c r="G14" s="160"/>
-      <c r="H14" s="161"/>
-      <c r="I14" s="162" t="s">
+      <c r="E15" s="159"/>
+      <c r="F15" s="159"/>
+      <c r="G15" s="160"/>
+      <c r="H15" s="161"/>
+      <c r="I15" s="162" t="s">
         <v>91</v>
       </c>
-      <c r="J14" s="163"/>
-      <c r="K14" s="224"/>
-    </row>
-    <row r="15" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="165"/>
-      <c r="C15" s="220" t="s">
+      <c r="J15" s="163"/>
+      <c r="K15" s="224"/>
+    </row>
+    <row r="16" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="220" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="226">
+      <c r="D16" s="226">
         <v>60</v>
       </c>
-      <c r="E15" s="166"/>
-      <c r="F15" s="166"/>
-      <c r="G15" s="167"/>
-      <c r="H15" s="168"/>
-      <c r="I15" s="221" t="s">
+      <c r="E16" s="166"/>
+      <c r="F16" s="166"/>
+      <c r="G16" s="167"/>
+      <c r="H16" s="168"/>
+      <c r="I16" s="221" t="s">
         <v>93</v>
       </c>
-      <c r="J15" s="169"/>
-      <c r="K15" s="17"/>
-    </row>
-    <row r="16" spans="1:22" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="107"/>
-      <c r="C16" s="222" t="s">
+      <c r="J16" s="169"/>
+      <c r="K16" s="17"/>
+    </row>
+    <row r="17" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="107"/>
+      <c r="C17" s="222" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="125">
+      <c r="D17" s="125">
         <v>60</v>
       </c>
-      <c r="E16" s="107"/>
-      <c r="F16" s="107"/>
-      <c r="G16" s="103"/>
-      <c r="H16" s="104"/>
-      <c r="I16" s="223" t="s">
+      <c r="E17" s="107"/>
+      <c r="F17" s="107"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="104"/>
+      <c r="I17" s="223" t="s">
         <v>95</v>
       </c>
-      <c r="J16" s="112"/>
-      <c r="K16" s="7"/>
-    </row>
-    <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="64"/>
-      <c r="C17" s="127" t="s">
+      <c r="J17" s="112"/>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="64"/>
+      <c r="C18" s="127" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="128">
+      <c r="D18" s="128">
         <f>SUM(D6+D12)</f>
         <v>21</v>
       </c>
-      <c r="E17" s="71">
-        <f>SUM((E13+'Sprint 2 xx.xx - xx.xx'!E13)/60)</f>
+      <c r="E18" s="71">
+        <f>SUM((E14+'Sprint 2 xx.xx - xx.xx'!E13)/60)</f>
         <v>6</v>
       </c>
-      <c r="F17" s="67"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="72"/>
-    </row>
-    <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="64"/>
-      <c r="C18" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="65">
-        <f>SUM(D17+D19)</f>
-        <v>23</v>
-      </c>
-      <c r="E18" s="65"/>
       <c r="F18" s="67"/>
       <c r="G18" s="68"/>
       <c r="H18" s="68"/>
       <c r="I18" s="69"/>
       <c r="J18" s="72"/>
     </row>
-    <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="64"/>
       <c r="C19" s="65" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="65">
-        <v>2</v>
+        <f>SUM(D18+D20)</f>
+        <v>23</v>
       </c>
       <c r="E19" s="65"/>
       <c r="F19" s="67"/>
       <c r="G19" s="68"/>
       <c r="H19" s="68"/>
       <c r="I19" s="69"/>
-      <c r="J19" s="47"/>
+      <c r="J19" s="72"/>
+    </row>
+    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="64"/>
+      <c r="C20" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="65">
+        <v>2</v>
+      </c>
+      <c r="E20" s="65"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="68"/>
+      <c r="I20" s="69"/>
+      <c r="J20" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
@@ -3893,8 +3919,8 @@
     <row r="1" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="74"/>
       <c r="D1" s="3"/>
-      <c r="G1" s="256"/>
-      <c r="H1" s="257"/>
+      <c r="G1" s="257"/>
+      <c r="H1" s="258"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -3955,30 +3981,30 @@
     <row r="5" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="79"/>
-      <c r="C5" s="234"/>
-      <c r="D5" s="234"/>
-      <c r="E5" s="235"/>
-      <c r="F5" s="235"/>
-      <c r="G5" s="236"/>
-      <c r="H5" s="237"/>
-      <c r="I5" s="235"/>
+      <c r="C5" s="233"/>
+      <c r="D5" s="233"/>
+      <c r="E5" s="234"/>
+      <c r="F5" s="234"/>
+      <c r="G5" s="235"/>
+      <c r="H5" s="236"/>
+      <c r="I5" s="234"/>
       <c r="J5" s="37"/>
       <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:22" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="233">
+      <c r="B6" s="232">
         <v>6</v>
       </c>
-      <c r="C6" s="242" t="s">
+      <c r="C6" s="241" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="243">
+      <c r="D6" s="242">
         <f>SUM(D7:D9)</f>
         <v>180</v>
       </c>
       <c r="E6" s="134"/>
       <c r="F6" s="134"/>
-      <c r="G6" s="241"/>
+      <c r="G6" s="240"/>
       <c r="H6" s="137"/>
       <c r="I6" s="139"/>
       <c r="J6" s="70"/>
@@ -4097,7 +4123,7 @@
       <c r="F13" s="191"/>
       <c r="G13" s="104"/>
       <c r="H13" s="104"/>
-      <c r="I13" s="228" t="s">
+      <c r="I13" s="227" t="s">
         <v>101</v>
       </c>
       <c r="J13" s="112"/>

</xml_diff>

<commit_message>
Added book searching to customer sites
</commit_message>
<xml_diff>
--- a/plans/scrum-planering.xlsx
+++ b/plans/scrum-planering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\2024\yrkesprov\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1028979C-3477-4A75-A6C1-0DE0D7E646A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F73A0E9-34E1-474F-B64B-CBDB6A3E46EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{41C2E65D-138E-4665-8AB5-B482A8FDA31A}"/>
   </bookViews>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="111">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -455,6 +455,12 @@
   </si>
   <si>
     <t>2/h 20/11/24                                   4/h 21/11/24 || Edit funkar till vissa saker, expandera senare</t>
+  </si>
+  <si>
+    <t>Livesearch byggnes in rakt I sökfunktionen</t>
+  </si>
+  <si>
+    <t>Kan från början söka på Författare samt tittel</t>
   </si>
 </sst>
 </file>
@@ -849,7 +855,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="261">
+  <cellXfs count="260">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1524,6 +1530,9 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1538,12 +1547,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2397,13 +2400,13 @@
   <sheetData>
     <row r="1" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="216"/>
-      <c r="B1" s="254" t="s">
+      <c r="B1" s="255" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="255"/>
-      <c r="D1" s="255"/>
-      <c r="E1" s="255"/>
-      <c r="F1" s="256"/>
+      <c r="C1" s="256"/>
+      <c r="D1" s="256"/>
+      <c r="E1" s="256"/>
+      <c r="F1" s="257"/>
     </row>
     <row r="2" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="216"/>
@@ -2675,10 +2678,10 @@
         <v>0</v>
       </c>
       <c r="D1" s="3"/>
-      <c r="G1" s="257" t="s">
+      <c r="G1" s="258" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="258"/>
+      <c r="H1" s="259"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="4"/>
@@ -3077,8 +3080,8 @@
     <row r="1" spans="1:22" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="74"/>
       <c r="D1" s="75"/>
-      <c r="G1" s="257"/>
-      <c r="H1" s="257"/>
+      <c r="G1" s="258"/>
+      <c r="H1" s="258"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -3507,8 +3510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C94DF7-B35F-4481-A77A-5670F6E3A59A}">
   <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3529,8 +3532,8 @@
     <row r="1" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="74"/>
       <c r="D1" s="3"/>
-      <c r="G1" s="257"/>
-      <c r="H1" s="258"/>
+      <c r="G1" s="258"/>
+      <c r="H1" s="259"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -3615,7 +3618,7 @@
       </c>
       <c r="E6" s="244">
         <f>SUM(E7:E13)/60</f>
-        <v>1.0333333333333334</v>
+        <v>6.0333333333333332</v>
       </c>
       <c r="F6" s="115"/>
       <c r="G6" s="116"/>
@@ -3647,7 +3650,7 @@
       </c>
       <c r="J7" s="231"/>
     </row>
-    <row r="8" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="104"/>
       <c r="C8" s="119" t="s">
@@ -3656,14 +3659,22 @@
       <c r="D8" s="120">
         <v>240</v>
       </c>
-      <c r="E8" s="121"/>
+      <c r="E8" s="121">
+        <v>300</v>
+      </c>
       <c r="F8" s="121"/>
-      <c r="G8" s="122"/>
-      <c r="H8" s="123"/>
+      <c r="G8" s="122" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="123">
+        <v>45622</v>
+      </c>
       <c r="I8" s="250" t="s">
         <v>79</v>
       </c>
-      <c r="J8" s="231"/>
+      <c r="J8" s="231" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="9" spans="1:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
@@ -3674,14 +3685,22 @@
       <c r="D9" s="120">
         <v>180</v>
       </c>
-      <c r="E9" s="73"/>
+      <c r="E9" s="73">
+        <v>0</v>
+      </c>
       <c r="F9" s="121"/>
-      <c r="G9" s="122"/>
-      <c r="H9" s="123"/>
+      <c r="G9" s="122" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="123">
+        <v>45622</v>
+      </c>
       <c r="I9" s="250" t="s">
         <v>78</v>
       </c>
-      <c r="J9" s="231"/>
+      <c r="J9" s="231" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="10" spans="1:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
@@ -3702,7 +3721,7 @@
       <c r="J10" s="104"/>
     </row>
     <row r="11" spans="1:22" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="259"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="231"/>
       <c r="C11" s="231"/>
       <c r="D11" s="94"/>
@@ -3721,7 +3740,7 @@
       <c r="C12" s="114" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="260">
+      <c r="D12" s="254">
         <f>SUM(D13:D17)/60</f>
         <v>9</v>
       </c>
@@ -3919,8 +3938,8 @@
     <row r="1" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="74"/>
       <c r="D1" s="3"/>
-      <c r="G1" s="257"/>
-      <c r="H1" s="258"/>
+      <c r="G1" s="258"/>
+      <c r="H1" s="259"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>

</xml_diff>

<commit_message>
delete user works and searching is finished
</commit_message>
<xml_diff>
--- a/plans/scrum-planering.xlsx
+++ b/plans/scrum-planering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\2024\yrkesprov\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F73A0E9-34E1-474F-B64B-CBDB6A3E46EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD0CCE4-1F28-423A-85B3-3907C9CF46D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{41C2E65D-138E-4665-8AB5-B482A8FDA31A}"/>
   </bookViews>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="111">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -855,7 +855,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="260">
+  <cellXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1189,9 +1189,6 @@
     </xf>
     <xf numFmtId="14" fontId="3" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2399,18 +2396,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="216"/>
-      <c r="B1" s="255" t="s">
+      <c r="A1" s="215"/>
+      <c r="B1" s="254" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="256"/>
-      <c r="D1" s="256"/>
-      <c r="E1" s="256"/>
-      <c r="F1" s="257"/>
+      <c r="C1" s="255"/>
+      <c r="D1" s="255"/>
+      <c r="E1" s="255"/>
+      <c r="F1" s="256"/>
     </row>
     <row r="2" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A2" s="216"/>
-      <c r="B2" s="218" t="s">
+      <c r="A2" s="215"/>
+      <c r="B2" s="217" t="s">
         <v>55</v>
       </c>
       <c r="C2" s="24" t="s">
@@ -2419,227 +2416,227 @@
       <c r="D2" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="216" t="s">
+      <c r="E2" s="215" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="217"/>
+      <c r="F2" s="216"/>
     </row>
     <row r="3" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="216"/>
-      <c r="B3" s="214" t="s">
+      <c r="A3" s="215"/>
+      <c r="B3" s="213" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="215" t="s">
+      <c r="C3" s="214" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="214"/>
-      <c r="E3" s="214" t="s">
+      <c r="D3" s="213"/>
+      <c r="E3" s="213" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="205"/>
+      <c r="F3" s="204"/>
     </row>
     <row r="4" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="195">
+      <c r="A4" s="194">
         <v>1</v>
       </c>
-      <c r="B4" s="212" t="s">
+      <c r="B4" s="211" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="207">
+      <c r="C4" s="206">
         <v>8</v>
       </c>
-      <c r="D4" s="195">
+      <c r="D4" s="194">
         <v>1</v>
       </c>
-      <c r="E4" s="206" t="s">
+      <c r="E4" s="205" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="205"/>
-      <c r="I4" s="213"/>
+      <c r="F4" s="204"/>
+      <c r="I4" s="212"/>
     </row>
     <row r="5" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="195">
+      <c r="A5" s="194">
         <v>2</v>
       </c>
-      <c r="B5" s="212" t="s">
+      <c r="B5" s="211" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="207">
+      <c r="C5" s="206">
         <v>5</v>
       </c>
-      <c r="D5" s="195">
+      <c r="D5" s="194">
         <v>2</v>
       </c>
-      <c r="E5" s="206" t="s">
+      <c r="E5" s="205" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="205"/>
+      <c r="F5" s="204"/>
     </row>
     <row r="6" spans="1:9" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="195">
+      <c r="A6" s="194">
         <v>4</v>
       </c>
-      <c r="B6" s="208" t="s">
+      <c r="B6" s="207" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="207">
+      <c r="C6" s="206">
         <v>14</v>
       </c>
-      <c r="D6" s="195">
+      <c r="D6" s="194">
         <v>4</v>
       </c>
-      <c r="E6" s="211" t="s">
+      <c r="E6" s="210" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="205"/>
+      <c r="F6" s="204"/>
     </row>
     <row r="7" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="195">
+      <c r="A7" s="194">
         <v>3</v>
       </c>
-      <c r="B7" s="209" t="s">
+      <c r="B7" s="208" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="207">
+      <c r="C7" s="206">
         <v>7</v>
       </c>
-      <c r="D7" s="195">
+      <c r="D7" s="194">
         <v>3</v>
       </c>
-      <c r="E7" s="210" t="s">
+      <c r="E7" s="209" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="205"/>
+      <c r="F7" s="204"/>
     </row>
     <row r="8" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="195">
+      <c r="A8" s="194">
         <v>5</v>
       </c>
-      <c r="B8" s="209" t="s">
+      <c r="B8" s="208" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="207">
+      <c r="C8" s="206">
         <v>6</v>
       </c>
-      <c r="D8" s="195">
+      <c r="D8" s="194">
         <v>8</v>
       </c>
-      <c r="E8" s="206" t="s">
+      <c r="E8" s="205" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="205"/>
+      <c r="F8" s="204"/>
     </row>
     <row r="9" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="195">
+      <c r="A9" s="194">
         <v>6</v>
       </c>
-      <c r="B9" s="209" t="s">
+      <c r="B9" s="208" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="73">
         <v>2</v>
       </c>
-      <c r="D9" s="195">
+      <c r="D9" s="194">
         <v>5</v>
       </c>
-      <c r="E9" s="206" t="s">
+      <c r="E9" s="205" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="205"/>
+      <c r="F9" s="204"/>
     </row>
     <row r="10" spans="1:9" ht="57.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="195">
+      <c r="A10" s="194">
         <v>7</v>
       </c>
-      <c r="B10" s="208" t="s">
+      <c r="B10" s="207" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="207">
+      <c r="C10" s="206">
         <v>1</v>
       </c>
-      <c r="D10" s="195">
+      <c r="D10" s="194">
         <v>7</v>
       </c>
-      <c r="E10" s="206" t="s">
+      <c r="E10" s="205" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="205"/>
+      <c r="F10" s="204"/>
     </row>
     <row r="11" spans="1:9" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="195">
+      <c r="A11" s="194">
         <v>8</v>
       </c>
-      <c r="B11" s="206" t="s">
+      <c r="B11" s="205" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="207">
+      <c r="C11" s="206">
         <v>1</v>
       </c>
-      <c r="D11" s="195">
+      <c r="D11" s="194">
         <v>6</v>
       </c>
-      <c r="E11" s="206" t="s">
+      <c r="E11" s="205" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="205"/>
+      <c r="F11" s="204"/>
     </row>
     <row r="12" spans="1:9" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="195">
+      <c r="A12" s="194">
         <v>9</v>
       </c>
-      <c r="B12" s="208" t="s">
+      <c r="B12" s="207" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="207">
+      <c r="C12" s="206">
         <v>3</v>
       </c>
-      <c r="D12" s="195">
+      <c r="D12" s="194">
         <v>9</v>
       </c>
-      <c r="E12" s="206" t="s">
+      <c r="E12" s="205" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="205"/>
+      <c r="F12" s="204"/>
     </row>
     <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="200"/>
-      <c r="B13" s="204"/>
-      <c r="C13" s="197"/>
-      <c r="D13" s="197"/>
-      <c r="E13" s="203"/>
-      <c r="F13" s="196"/>
+      <c r="A13" s="199"/>
+      <c r="B13" s="203"/>
+      <c r="C13" s="196"/>
+      <c r="D13" s="196"/>
+      <c r="E13" s="202"/>
+      <c r="F13" s="195"/>
     </row>
     <row r="14" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="200"/>
-      <c r="B14" s="203"/>
-      <c r="C14" s="203"/>
-      <c r="D14" s="203"/>
-      <c r="E14" s="203"/>
-      <c r="F14" s="196"/>
+      <c r="A14" s="199"/>
+      <c r="B14" s="202"/>
+      <c r="C14" s="202"/>
+      <c r="D14" s="202"/>
+      <c r="E14" s="202"/>
+      <c r="F14" s="195"/>
     </row>
     <row r="15" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="202"/>
-      <c r="B15" s="203"/>
-      <c r="C15" s="202"/>
-      <c r="D15" s="202"/>
-      <c r="E15" s="201"/>
-      <c r="F15" s="196"/>
+      <c r="A15" s="201"/>
+      <c r="B15" s="202"/>
+      <c r="C15" s="201"/>
+      <c r="D15" s="201"/>
+      <c r="E15" s="200"/>
+      <c r="F15" s="195"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="200"/>
-      <c r="B16" s="199" t="s">
+      <c r="A16" s="199"/>
+      <c r="B16" s="198" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="198">
+      <c r="C16" s="197">
         <f>SUM(C4:C15)</f>
         <v>47</v>
       </c>
-      <c r="D16" s="197"/>
-      <c r="E16" s="197">
+      <c r="D16" s="196"/>
+      <c r="E16" s="196">
         <f>C16*60</f>
         <v>2820</v>
       </c>
-      <c r="F16" s="196"/>
+      <c r="F16" s="195"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2678,10 +2675,10 @@
         <v>0</v>
       </c>
       <c r="D1" s="3"/>
-      <c r="G1" s="258" t="s">
+      <c r="G1" s="257" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="259"/>
+      <c r="H1" s="258"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="4"/>
@@ -2766,7 +2763,7 @@
         <f>SUM(D7:D13) / 60</f>
         <v>7.75</v>
       </c>
-      <c r="E6" s="229">
+      <c r="E6" s="228">
         <f>SUM(E7:E13)/60</f>
         <v>13.25</v>
       </c>
@@ -2796,7 +2793,7 @@
       <c r="H7" s="54">
         <v>45604</v>
       </c>
-      <c r="I7" s="219" t="s">
+      <c r="I7" s="218" t="s">
         <v>63</v>
       </c>
       <c r="J7" s="56"/>
@@ -2821,7 +2818,7 @@
       <c r="H8" s="54">
         <v>45608</v>
       </c>
-      <c r="I8" s="219" t="s">
+      <c r="I8" s="218" t="s">
         <v>64</v>
       </c>
       <c r="J8" s="56"/>
@@ -2848,7 +2845,7 @@
       <c r="H9" s="54">
         <v>45607</v>
       </c>
-      <c r="I9" s="219" t="s">
+      <c r="I9" s="218" t="s">
         <v>65</v>
       </c>
       <c r="J9" s="56"/>
@@ -2875,7 +2872,7 @@
       <c r="H10" s="54">
         <v>45607</v>
       </c>
-      <c r="I10" s="219" t="s">
+      <c r="I10" s="218" t="s">
         <v>66</v>
       </c>
       <c r="J10" s="56"/>
@@ -2900,10 +2897,10 @@
       <c r="H11" s="54">
         <v>45609</v>
       </c>
-      <c r="I11" s="219" t="s">
+      <c r="I11" s="218" t="s">
         <v>67</v>
       </c>
-      <c r="J11" s="228"/>
+      <c r="J11" s="227"/>
       <c r="K11" s="62"/>
     </row>
     <row r="12" spans="1:22" ht="61.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2925,7 +2922,7 @@
       <c r="H12" s="54">
         <v>45610</v>
       </c>
-      <c r="I12" s="219" t="s">
+      <c r="I12" s="218" t="s">
         <v>62</v>
       </c>
       <c r="J12" s="56"/>
@@ -2950,7 +2947,7 @@
       <c r="H13" s="54">
         <v>45607</v>
       </c>
-      <c r="I13" s="219" t="s">
+      <c r="I13" s="218" t="s">
         <v>68</v>
       </c>
       <c r="J13" s="56"/>
@@ -3058,7 +3055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF3BD90-0203-44B4-AE4B-CE188AD45574}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
@@ -3080,8 +3077,8 @@
     <row r="1" spans="1:22" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="74"/>
       <c r="D1" s="75"/>
-      <c r="G1" s="258"/>
-      <c r="H1" s="258"/>
+      <c r="G1" s="257"/>
+      <c r="H1" s="257"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -3142,36 +3139,36 @@
     <row r="5" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="79"/>
-      <c r="C5" s="233"/>
-      <c r="D5" s="233"/>
-      <c r="E5" s="234"/>
-      <c r="F5" s="234"/>
-      <c r="G5" s="235"/>
-      <c r="H5" s="236"/>
-      <c r="I5" s="234"/>
+      <c r="C5" s="232"/>
+      <c r="D5" s="232"/>
+      <c r="E5" s="233"/>
+      <c r="F5" s="233"/>
+      <c r="G5" s="234"/>
+      <c r="H5" s="235"/>
+      <c r="I5" s="233"/>
       <c r="J5" s="37"/>
       <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:22" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38"/>
-      <c r="B6" s="232">
+      <c r="B6" s="231">
         <v>2</v>
       </c>
-      <c r="C6" s="238" t="s">
+      <c r="C6" s="237" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="239">
+      <c r="D6" s="238">
         <f>SUM(D7:D11)/60</f>
         <v>3.5</v>
       </c>
-      <c r="E6" s="245">
+      <c r="E6" s="244">
         <f>SUM(E7:E11)/60</f>
         <v>3</v>
       </c>
-      <c r="F6" s="134"/>
-      <c r="G6" s="240"/>
-      <c r="H6" s="137"/>
-      <c r="I6" s="139"/>
+      <c r="F6" s="133"/>
+      <c r="G6" s="239"/>
+      <c r="H6" s="136"/>
+      <c r="I6" s="138"/>
       <c r="J6" s="47"/>
       <c r="K6" s="7"/>
     </row>
@@ -3191,7 +3188,7 @@
       <c r="G7" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="237">
+      <c r="H7" s="236">
         <v>45610</v>
       </c>
       <c r="I7" s="87" t="s">
@@ -3269,7 +3266,7 @@
       <c r="H10" s="97">
         <v>45611</v>
       </c>
-      <c r="I10" s="192" t="s">
+      <c r="I10" s="191" t="s">
         <v>72</v>
       </c>
       <c r="J10" s="104"/>
@@ -3294,7 +3291,7 @@
       <c r="H11" s="54">
         <v>45610</v>
       </c>
-      <c r="I11" s="192" t="s">
+      <c r="I11" s="191" t="s">
         <v>73</v>
       </c>
       <c r="J11" s="104"/>
@@ -3312,15 +3309,15 @@
         <f>SUM(D13:D15)/60</f>
         <v>7</v>
       </c>
-      <c r="E12" s="244">
+      <c r="E12" s="243">
         <f>SUM(E13:E17)/60</f>
         <v>7</v>
       </c>
       <c r="F12" s="115"/>
       <c r="G12" s="116"/>
-      <c r="H12" s="150"/>
-      <c r="I12" s="151"/>
-      <c r="J12" s="152"/>
+      <c r="H12" s="149"/>
+      <c r="I12" s="150"/>
+      <c r="J12" s="151"/>
       <c r="K12" s="17"/>
     </row>
     <row r="13" spans="1:22" ht="13.8" x14ac:dyDescent="0.25">
@@ -3332,17 +3329,17 @@
       <c r="D13" s="120">
         <v>120</v>
       </c>
-      <c r="E13" s="252">
+      <c r="E13" s="251">
         <v>360</v>
       </c>
       <c r="F13" s="121"/>
-      <c r="G13" s="243" t="s">
+      <c r="G13" s="242" t="s">
         <v>14</v>
       </c>
       <c r="H13" s="123">
         <v>45615</v>
       </c>
-      <c r="I13" s="153" t="s">
+      <c r="I13" s="152" t="s">
         <v>84</v>
       </c>
       <c r="J13" s="104" t="s">
@@ -3359,7 +3356,7 @@
       <c r="D14" s="120">
         <v>120</v>
       </c>
-      <c r="E14" s="252">
+      <c r="E14" s="251">
         <v>60</v>
       </c>
       <c r="F14" s="121"/>
@@ -3369,7 +3366,7 @@
       <c r="H14" s="123">
         <v>45616</v>
       </c>
-      <c r="I14" s="153" t="s">
+      <c r="I14" s="152" t="s">
         <v>87</v>
       </c>
       <c r="J14" s="104"/>
@@ -3378,7 +3375,7 @@
     <row r="15" spans="1:22" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="104"/>
-      <c r="C15" s="154" t="s">
+      <c r="C15" s="153" t="s">
         <v>89</v>
       </c>
       <c r="D15" s="120">
@@ -3388,62 +3385,62 @@
       <c r="F15" s="121"/>
       <c r="G15" s="107"/>
       <c r="H15" s="107"/>
-      <c r="I15" s="153" t="s">
+      <c r="I15" s="152" t="s">
         <v>88</v>
       </c>
-      <c r="J15" s="192" t="s">
+      <c r="J15" s="191" t="s">
         <v>108</v>
       </c>
       <c r="K15" s="17"/>
     </row>
     <row r="16" spans="1:22" ht="19.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
-      <c r="B16" s="231"/>
-      <c r="C16" s="231"/>
-      <c r="D16" s="231"/>
-      <c r="E16" s="231"/>
-      <c r="F16" s="231"/>
-      <c r="G16" s="231"/>
-      <c r="H16" s="231"/>
-      <c r="I16" s="231"/>
+      <c r="B16" s="230"/>
+      <c r="C16" s="230"/>
+      <c r="D16" s="230"/>
+      <c r="E16" s="230"/>
+      <c r="F16" s="230"/>
+      <c r="G16" s="230"/>
+      <c r="H16" s="230"/>
+      <c r="I16" s="230"/>
       <c r="J16" s="104"/>
       <c r="K16" s="17"/>
     </row>
     <row r="17" spans="1:11" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
-      <c r="B17" s="231"/>
-      <c r="C17" s="231"/>
-      <c r="D17" s="231"/>
-      <c r="E17" s="231"/>
-      <c r="F17" s="231"/>
-      <c r="G17" s="231"/>
-      <c r="H17" s="231"/>
-      <c r="I17" s="231"/>
+      <c r="B17" s="230"/>
+      <c r="C17" s="230"/>
+      <c r="D17" s="230"/>
+      <c r="E17" s="230"/>
+      <c r="F17" s="230"/>
+      <c r="G17" s="230"/>
+      <c r="H17" s="230"/>
+      <c r="I17" s="230"/>
       <c r="J17" s="112"/>
       <c r="K17" s="7"/>
     </row>
     <row r="18" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38"/>
-      <c r="B18" s="126"/>
-      <c r="C18" s="246" t="s">
+      <c r="B18" s="125"/>
+      <c r="C18" s="245" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="247">
+      <c r="D18" s="246">
         <f>SUM(D6+D12)</f>
         <v>10.5</v>
       </c>
-      <c r="E18" s="253">
+      <c r="E18" s="252">
         <f>SUM(E6+E12)</f>
         <v>10</v>
       </c>
-      <c r="F18" s="248"/>
-      <c r="G18" s="126"/>
-      <c r="H18" s="126"/>
-      <c r="I18" s="126"/>
+      <c r="F18" s="247"/>
+      <c r="G18" s="125"/>
+      <c r="H18" s="125"/>
+      <c r="I18" s="125"/>
       <c r="J18" s="70"/>
     </row>
     <row r="19" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="129"/>
+      <c r="B19" s="128"/>
       <c r="C19" s="80" t="s">
         <v>24</v>
       </c>
@@ -3451,49 +3448,49 @@
         <f>SUM(D20+D18)</f>
         <v>13</v>
       </c>
-      <c r="E19" s="130"/>
-      <c r="F19" s="131"/>
+      <c r="E19" s="129"/>
+      <c r="F19" s="130"/>
       <c r="G19" s="45"/>
       <c r="H19" s="45"/>
-      <c r="I19" s="132"/>
+      <c r="I19" s="131"/>
       <c r="J19" s="72"/>
     </row>
     <row r="20" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="133"/>
-      <c r="C20" s="134" t="s">
+      <c r="B20" s="132"/>
+      <c r="C20" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="230">
+      <c r="D20" s="229">
         <v>2.5</v>
       </c>
-      <c r="E20" s="135"/>
-      <c r="F20" s="136"/>
-      <c r="G20" s="137"/>
-      <c r="H20" s="137"/>
-      <c r="I20" s="138"/>
-      <c r="J20" s="139"/>
+      <c r="E20" s="134"/>
+      <c r="F20" s="135"/>
+      <c r="G20" s="136"/>
+      <c r="H20" s="136"/>
+      <c r="I20" s="137"/>
+      <c r="J20" s="138"/>
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="140"/>
-      <c r="C21" s="141"/>
-      <c r="D21" s="141"/>
-      <c r="E21" s="142"/>
-      <c r="F21" s="143"/>
-      <c r="G21" s="144"/>
-      <c r="H21" s="144"/>
-      <c r="I21" s="145"/>
-      <c r="J21" s="146"/>
+      <c r="B21" s="139"/>
+      <c r="C21" s="140"/>
+      <c r="D21" s="140"/>
+      <c r="E21" s="141"/>
+      <c r="F21" s="142"/>
+      <c r="G21" s="143"/>
+      <c r="H21" s="143"/>
+      <c r="I21" s="144"/>
+      <c r="J21" s="145"/>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="147"/>
-      <c r="C22" s="141"/>
-      <c r="D22" s="141"/>
-      <c r="E22" s="142"/>
-      <c r="F22" s="143"/>
-      <c r="G22" s="144"/>
-      <c r="H22" s="144"/>
-      <c r="I22" s="145"/>
-      <c r="J22" s="146"/>
+      <c r="B22" s="146"/>
+      <c r="C22" s="140"/>
+      <c r="D22" s="140"/>
+      <c r="E22" s="141"/>
+      <c r="F22" s="142"/>
+      <c r="G22" s="143"/>
+      <c r="H22" s="143"/>
+      <c r="I22" s="144"/>
+      <c r="J22" s="145"/>
     </row>
     <row r="31" spans="1:11" ht="13.2" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -3510,8 +3507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C94DF7-B35F-4481-A77A-5670F6E3A59A}">
   <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3532,8 +3529,8 @@
     <row r="1" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="74"/>
       <c r="D1" s="3"/>
-      <c r="G1" s="258"/>
-      <c r="H1" s="259"/>
+      <c r="G1" s="257"/>
+      <c r="H1" s="258"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -3558,7 +3555,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="78"/>
       <c r="J3" s="16"/>
-      <c r="K3" s="148"/>
+      <c r="K3" s="147"/>
     </row>
     <row r="4" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
@@ -3574,7 +3571,7 @@
       <c r="E4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="149" t="s">
+      <c r="F4" s="148" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="24" t="s">
@@ -3601,7 +3598,7 @@
       <c r="G5" s="34"/>
       <c r="H5" s="35"/>
       <c r="I5" s="32"/>
-      <c r="J5" s="251"/>
+      <c r="J5" s="250"/>
       <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:22" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -3616,20 +3613,20 @@
         <f>SUM(D7:D10)/60</f>
         <v>12</v>
       </c>
-      <c r="E6" s="244">
+      <c r="E6" s="243">
         <f>SUM(E7:E13)/60</f>
-        <v>6.0333333333333332</v>
+        <v>6.5333333333333332</v>
       </c>
       <c r="F6" s="115"/>
       <c r="G6" s="116"/>
       <c r="H6" s="117"/>
-      <c r="I6" s="249"/>
-      <c r="J6" s="231"/>
+      <c r="I6" s="248"/>
+      <c r="J6" s="230"/>
     </row>
     <row r="7" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="104"/>
-      <c r="C7" s="213" t="s">
+      <c r="C7" s="212" t="s">
         <v>104</v>
       </c>
       <c r="D7" s="109">
@@ -3639,16 +3636,16 @@
         <v>60</v>
       </c>
       <c r="F7" s="121"/>
-      <c r="G7" s="243" t="s">
+      <c r="G7" s="242" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="123">
         <v>45611</v>
       </c>
-      <c r="I7" s="213" t="s">
+      <c r="I7" s="212" t="s">
         <v>105</v>
       </c>
-      <c r="J7" s="231"/>
+      <c r="J7" s="230"/>
     </row>
     <row r="8" spans="1:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
@@ -3669,10 +3666,10 @@
       <c r="H8" s="123">
         <v>45622</v>
       </c>
-      <c r="I8" s="250" t="s">
+      <c r="I8" s="249" t="s">
         <v>79</v>
       </c>
-      <c r="J8" s="231" t="s">
+      <c r="J8" s="230" t="s">
         <v>110</v>
       </c>
     </row>
@@ -3695,10 +3692,10 @@
       <c r="H9" s="123">
         <v>45622</v>
       </c>
-      <c r="I9" s="250" t="s">
+      <c r="I9" s="249" t="s">
         <v>78</v>
       </c>
-      <c r="J9" s="231" t="s">
+      <c r="J9" s="230" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3711,26 +3708,32 @@
       <c r="D10" s="102">
         <v>180</v>
       </c>
-      <c r="E10" s="103"/>
+      <c r="E10" s="103">
+        <v>30</v>
+      </c>
       <c r="F10" s="104"/>
-      <c r="G10" s="105"/>
-      <c r="H10" s="124"/>
-      <c r="I10" s="192" t="s">
+      <c r="G10" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="97">
+        <v>45628</v>
+      </c>
+      <c r="I10" s="191" t="s">
         <v>81</v>
       </c>
       <c r="J10" s="104"/>
     </row>
     <row r="11" spans="1:22" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="231"/>
-      <c r="C11" s="231"/>
+      <c r="B11" s="230"/>
+      <c r="C11" s="230"/>
       <c r="D11" s="94"/>
-      <c r="E11" s="231"/>
-      <c r="F11" s="231"/>
-      <c r="G11" s="231"/>
-      <c r="H11" s="231"/>
-      <c r="I11" s="231"/>
-      <c r="J11" s="231"/>
+      <c r="E11" s="230"/>
+      <c r="F11" s="230"/>
+      <c r="G11" s="230"/>
+      <c r="H11" s="230"/>
+      <c r="I11" s="230"/>
+      <c r="J11" s="230"/>
     </row>
     <row r="12" spans="1:22" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
@@ -3740,15 +3743,15 @@
       <c r="C12" s="114" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="254">
+      <c r="D12" s="253">
         <f>SUM(D13:D17)/60</f>
         <v>9</v>
       </c>
       <c r="E12" s="115"/>
       <c r="F12" s="115"/>
-      <c r="G12" s="155"/>
-      <c r="H12" s="155"/>
-      <c r="I12" s="151"/>
+      <c r="G12" s="154"/>
+      <c r="H12" s="154"/>
+      <c r="I12" s="150"/>
       <c r="J12" s="118"/>
     </row>
     <row r="13" spans="1:22" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
@@ -3770,7 +3773,7 @@
       <c r="H13" s="97">
         <v>45621</v>
       </c>
-      <c r="I13" s="225" t="s">
+      <c r="I13" s="224" t="s">
         <v>74</v>
       </c>
       <c r="J13" s="104"/>
@@ -3781,7 +3784,7 @@
       <c r="C14" s="119" t="s">
         <v>96</v>
       </c>
-      <c r="D14" s="225">
+      <c r="D14" s="224">
         <v>180</v>
       </c>
       <c r="E14" s="121"/>
@@ -3792,60 +3795,60 @@
         <v>97</v>
       </c>
       <c r="J14" s="112"/>
-      <c r="K14" s="164"/>
+      <c r="K14" s="163"/>
     </row>
     <row r="15" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
-      <c r="B15" s="156"/>
-      <c r="C15" s="157" t="s">
+      <c r="B15" s="155"/>
+      <c r="C15" s="156" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="158">
+      <c r="D15" s="157">
         <v>120</v>
       </c>
-      <c r="E15" s="159"/>
-      <c r="F15" s="159"/>
-      <c r="G15" s="160"/>
-      <c r="H15" s="161"/>
-      <c r="I15" s="162" t="s">
+      <c r="E15" s="158"/>
+      <c r="F15" s="158"/>
+      <c r="G15" s="159"/>
+      <c r="H15" s="160"/>
+      <c r="I15" s="161" t="s">
         <v>91</v>
       </c>
-      <c r="J15" s="163"/>
-      <c r="K15" s="224"/>
+      <c r="J15" s="162"/>
+      <c r="K15" s="223"/>
     </row>
     <row r="16" spans="1:22" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
-      <c r="B16" s="165"/>
-      <c r="C16" s="220" t="s">
+      <c r="B16" s="164"/>
+      <c r="C16" s="219" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="226">
+      <c r="D16" s="225">
         <v>60</v>
       </c>
-      <c r="E16" s="166"/>
-      <c r="F16" s="166"/>
-      <c r="G16" s="167"/>
-      <c r="H16" s="168"/>
-      <c r="I16" s="221" t="s">
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="166"/>
+      <c r="H16" s="167"/>
+      <c r="I16" s="220" t="s">
         <v>93</v>
       </c>
-      <c r="J16" s="169"/>
+      <c r="J16" s="168"/>
       <c r="K16" s="17"/>
     </row>
     <row r="17" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="107"/>
-      <c r="C17" s="222" t="s">
+      <c r="C17" s="221" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="125">
+      <c r="D17" s="124">
         <v>60</v>
       </c>
       <c r="E17" s="107"/>
       <c r="F17" s="107"/>
       <c r="G17" s="103"/>
       <c r="H17" s="104"/>
-      <c r="I17" s="223" t="s">
+      <c r="I17" s="222" t="s">
         <v>95</v>
       </c>
       <c r="J17" s="112"/>
@@ -3853,10 +3856,10 @@
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="64"/>
-      <c r="C18" s="127" t="s">
+      <c r="C18" s="126" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="128">
+      <c r="D18" s="127">
         <f>SUM(D6+D12)</f>
         <v>21</v>
       </c>
@@ -3938,8 +3941,8 @@
     <row r="1" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="74"/>
       <c r="D1" s="3"/>
-      <c r="G1" s="258"/>
-      <c r="H1" s="259"/>
+      <c r="G1" s="257"/>
+      <c r="H1" s="258"/>
     </row>
     <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -3964,7 +3967,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="78"/>
       <c r="J3" s="16"/>
-      <c r="K3" s="148"/>
+      <c r="K3" s="147"/>
     </row>
     <row r="4" spans="1:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
@@ -4000,37 +4003,37 @@
     <row r="5" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="79"/>
-      <c r="C5" s="233"/>
-      <c r="D5" s="233"/>
-      <c r="E5" s="234"/>
-      <c r="F5" s="234"/>
-      <c r="G5" s="235"/>
-      <c r="H5" s="236"/>
-      <c r="I5" s="234"/>
+      <c r="C5" s="232"/>
+      <c r="D5" s="232"/>
+      <c r="E5" s="233"/>
+      <c r="F5" s="233"/>
+      <c r="G5" s="234"/>
+      <c r="H5" s="235"/>
+      <c r="I5" s="233"/>
       <c r="J5" s="37"/>
       <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:22" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="232">
+      <c r="B6" s="231">
         <v>6</v>
       </c>
-      <c r="C6" s="241" t="s">
+      <c r="C6" s="240" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="242">
+      <c r="D6" s="241">
         <f>SUM(D7:D9)</f>
         <v>180</v>
       </c>
-      <c r="E6" s="134"/>
-      <c r="F6" s="134"/>
-      <c r="G6" s="240"/>
-      <c r="H6" s="137"/>
-      <c r="I6" s="139"/>
+      <c r="E6" s="133"/>
+      <c r="F6" s="133"/>
+      <c r="G6" s="239"/>
+      <c r="H6" s="136"/>
+      <c r="I6" s="138"/>
       <c r="J6" s="70"/>
     </row>
     <row r="7" spans="1:22" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="170"/>
-      <c r="C7" s="171" t="s">
+      <c r="B7" s="169"/>
+      <c r="C7" s="170" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="84">
@@ -4038,15 +4041,15 @@
       </c>
       <c r="E7" s="85"/>
       <c r="F7" s="85"/>
-      <c r="G7" s="172"/>
-      <c r="H7" s="173"/>
-      <c r="I7" s="174" t="s">
+      <c r="G7" s="171"/>
+      <c r="H7" s="172"/>
+      <c r="I7" s="173" t="s">
         <v>107</v>
       </c>
       <c r="J7" s="99"/>
     </row>
     <row r="8" spans="1:22" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="170"/>
+      <c r="B8" s="169"/>
       <c r="C8" s="55" t="s">
         <v>36</v>
       </c>
@@ -4060,10 +4063,10 @@
       <c r="I8" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="J8" s="175"/>
+      <c r="J8" s="174"/>
     </row>
     <row r="9" spans="1:22" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="170"/>
+      <c r="B9" s="169"/>
       <c r="C9" s="55" t="s">
         <v>37</v>
       </c>
@@ -4080,24 +4083,24 @@
       <c r="J9" s="16"/>
     </row>
     <row r="10" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="176">
+      <c r="B10" s="175">
         <v>7</v>
       </c>
-      <c r="C10" s="177" t="s">
+      <c r="C10" s="176" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="178">
+      <c r="D10" s="177">
         <v>60</v>
       </c>
-      <c r="E10" s="179"/>
-      <c r="F10" s="179"/>
-      <c r="G10" s="180"/>
-      <c r="H10" s="180"/>
-      <c r="I10" s="181"/>
-      <c r="J10" s="182"/>
+      <c r="E10" s="178"/>
+      <c r="F10" s="178"/>
+      <c r="G10" s="179"/>
+      <c r="H10" s="179"/>
+      <c r="I10" s="180"/>
+      <c r="J10" s="181"/>
     </row>
     <row r="11" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="183"/>
+      <c r="B11" s="182"/>
       <c r="C11" s="55" t="s">
         <v>38</v>
       </c>
@@ -4114,59 +4117,59 @@
       <c r="J11" s="99"/>
     </row>
     <row r="12" spans="1:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="176">
+      <c r="B12" s="175">
         <v>8</v>
       </c>
-      <c r="C12" s="184" t="s">
+      <c r="C12" s="183" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="185">
+      <c r="D12" s="184">
         <v>60</v>
       </c>
-      <c r="E12" s="186"/>
-      <c r="F12" s="186"/>
-      <c r="G12" s="187"/>
-      <c r="H12" s="187"/>
-      <c r="I12" s="188"/>
-      <c r="J12" s="189"/>
+      <c r="E12" s="185"/>
+      <c r="F12" s="185"/>
+      <c r="G12" s="186"/>
+      <c r="H12" s="186"/>
+      <c r="I12" s="187"/>
+      <c r="J12" s="188"/>
     </row>
     <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="104"/>
-      <c r="C13" s="190" t="s">
+      <c r="C13" s="189" t="s">
         <v>39</v>
       </c>
       <c r="D13" s="110">
         <v>60</v>
       </c>
-      <c r="E13" s="191"/>
-      <c r="F13" s="191"/>
+      <c r="E13" s="190"/>
+      <c r="F13" s="190"/>
       <c r="G13" s="104"/>
       <c r="H13" s="104"/>
-      <c r="I13" s="227" t="s">
+      <c r="I13" s="226" t="s">
         <v>101</v>
       </c>
       <c r="J13" s="112"/>
     </row>
     <row r="14" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="155">
+      <c r="B14" s="154">
         <v>9</v>
       </c>
-      <c r="C14" s="193" t="s">
+      <c r="C14" s="192" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="116">
         <v>120</v>
       </c>
-      <c r="E14" s="155"/>
-      <c r="F14" s="155"/>
-      <c r="G14" s="194"/>
+      <c r="E14" s="154"/>
+      <c r="F14" s="154"/>
+      <c r="G14" s="193"/>
       <c r="H14" s="118"/>
-      <c r="I14" s="152"/>
-      <c r="J14" s="152"/>
+      <c r="I14" s="151"/>
+      <c r="J14" s="151"/>
     </row>
     <row r="15" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B15" s="170"/>
-      <c r="C15" s="171" t="s">
+      <c r="B15" s="169"/>
+      <c r="C15" s="170" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="84">
@@ -4174,13 +4177,13 @@
       </c>
       <c r="E15" s="85"/>
       <c r="F15" s="85"/>
-      <c r="G15" s="172"/>
-      <c r="H15" s="173"/>
-      <c r="I15" s="174"/>
+      <c r="G15" s="171"/>
+      <c r="H15" s="172"/>
+      <c r="I15" s="173"/>
       <c r="J15" s="99"/>
     </row>
     <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="170"/>
+      <c r="B16" s="169"/>
       <c r="C16" s="90"/>
       <c r="D16" s="50"/>
       <c r="E16" s="51"/>
@@ -4188,11 +4191,11 @@
       <c r="G16" s="60"/>
       <c r="H16" s="20"/>
       <c r="I16" s="90"/>
-      <c r="J16" s="175"/>
+      <c r="J16" s="174"/>
     </row>
     <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="64"/>
-      <c r="C17" s="127" t="s">
+      <c r="C17" s="126" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="65">
@@ -4214,7 +4217,7 @@
       <c r="C18" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="127"/>
+      <c r="D18" s="126"/>
       <c r="E18" s="65"/>
       <c r="F18" s="67"/>
       <c r="G18" s="68"/>

</xml_diff>

<commit_message>
Book editing works now
</commit_message>
<xml_diff>
--- a/plans/scrum-planering.xlsx
+++ b/plans/scrum-planering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\2024\yrkesprov\plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD0CCE4-1F28-423A-85B3-3907C9CF46D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0812E70-7681-4225-AD46-E4B26A8E855E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{41C2E65D-138E-4665-8AB5-B482A8FDA31A}"/>
   </bookViews>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="111">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -855,7 +855,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="259">
+  <cellXfs count="260">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1544,6 +1544,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3055,8 +3058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF3BD90-0203-44B4-AE4B-CE188AD45574}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3311,7 +3314,7 @@
       </c>
       <c r="E12" s="243">
         <f>SUM(E13:E17)/60</f>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F12" s="115"/>
       <c r="G12" s="116"/>
@@ -3381,10 +3384,16 @@
       <c r="D15" s="120">
         <v>180</v>
       </c>
-      <c r="E15" s="121"/>
+      <c r="E15" s="121">
+        <v>480</v>
+      </c>
       <c r="F15" s="121"/>
-      <c r="G15" s="107"/>
-      <c r="H15" s="107"/>
+      <c r="G15" s="107" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="123">
+        <v>45628</v>
+      </c>
       <c r="I15" s="152" t="s">
         <v>88</v>
       </c>
@@ -3431,7 +3440,7 @@
       </c>
       <c r="E18" s="252">
         <f>SUM(E6+E12)</f>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F18" s="247"/>
       <c r="G18" s="125"/>
@@ -3507,8 +3516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C94DF7-B35F-4481-A77A-5670F6E3A59A}">
   <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3613,9 +3622,9 @@
         <f>SUM(D7:D10)/60</f>
         <v>12</v>
       </c>
-      <c r="E6" s="243">
-        <f>SUM(E7:E13)/60</f>
-        <v>6.5333333333333332</v>
+      <c r="E6" s="259">
+        <f>SUM(E7:E11)/60</f>
+        <v>6.5</v>
       </c>
       <c r="F6" s="115"/>
       <c r="G6" s="116"/>
@@ -3747,7 +3756,10 @@
         <f>SUM(D13:D17)/60</f>
         <v>9</v>
       </c>
-      <c r="E12" s="115"/>
+      <c r="E12" s="115">
+        <f>SUM(E13:E17)/60</f>
+        <v>2</v>
+      </c>
       <c r="F12" s="115"/>
       <c r="G12" s="154"/>
       <c r="H12" s="154"/>
@@ -3764,7 +3776,7 @@
         <v>120</v>
       </c>
       <c r="E13" s="110">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="F13" s="107"/>
       <c r="G13" s="111" t="s">
@@ -3864,8 +3876,8 @@
         <v>21</v>
       </c>
       <c r="E18" s="71">
-        <f>SUM((E14+'Sprint 2 xx.xx - xx.xx'!E13)/60)</f>
-        <v>6</v>
+        <f>SUM(E6+E12)</f>
+        <v>8.5</v>
       </c>
       <c r="F18" s="67"/>
       <c r="G18" s="68"/>

</xml_diff>